<commit_message>
rerun the math50,math401 results
</commit_message>
<xml_diff>
--- a/data/math401/results/math401_eval_result.xlsx
+++ b/data/math401/results/math401_eval_result.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 2.0, 18: 1.0, 19: 0.0, 20: 0.0, 21: 10, 22: 0.0, 23: 0.0, 24: 2.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.11235955056179775, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 2.0, 42: 0.0, 43: 2.1451612903225805, 44: 0.0, 45: 2.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 2.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.39457459926017263, 65: 2.0, 66: 0.0, 67: 0.0, 68: 0.030534351145038167, 69: 0.06354916067146282, 70: 0.011111111111111112, 71: 0.0, 72: 0.0, 73: 2.0408163265306123, 74: 0.25125628140703515, 75: 0.0, 76: 0.999998998676325, 77: 0.02153187663163325, 78: 0.037101445219012985, 79: 0.3805124972361365, 80: 8.880656074963407e-07, 81: 0.010091379192163377, 82: 9.022857573128268e-08, 83: 0.8370729758925709, 84: 5.265504730000651e-08, 85: 8.574319808160072e-07, 86: 6.468847827153158e-06, 87: 0.32084993258895805, 88: 0.4501898090856154, 89: 10, 90: 10, 91: 10, 92: 10, 93: 10, 94: 10, 95: 10, 96: 10, 97: 10, 98: 10, 99: 10, 100: 10, 101: 0.0, 102: 0.0, 103: 1.5, 104: 1.0, 105: 1.75, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 10.0, 114: 0.6153846153846154, 115: 0.8, 116: 0.0, 117: 2.0, 118: 1.25, 119: 1.0909090909090908, 120: 0.0, 121: 0.9333333333333333, 122: 0.2222222222222222, 123: 2.0, 124: 0.9090909090909091, 125: 0.36363636363636365, 126: 0.0, 127: 0.006900000000000017, 128: 1.9989761965702586, 129: 0.0004043818637006199, 130: 0.007400000000000018, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.001920347332387049, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 2.0, 140: 0.0010000000000000009, 141: 0.3, 142: 2.0, 143: 1.6710526315789473, 144: 0.02, 145: 0.37999999999999995, 146: 0.625, 147: 0.0, 148: 0.0004852353391394181, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.018018018018018018, 154: 0.0, 155: 8.181818181818182, 156: 0.07177033492822966, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.018674136321195144, 161: 0.016722408026755852, 162: 0.020050125313283207, 163: 0.004553734061930784, 164: 0.02145002145002145, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.006064281382656155, 169: 0.014892032762472078, 170: 0.002932551319648094, 171: 0.0, 172: 0.0, 173: 0.012077294685990338, 174: 0.026954177897574125, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 8.1, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 10, 188: 10, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 9.001436454429912, 202: 0.000408557836845193, 204: 0.8986934250700569, 205: 0.9000933928425443, 206: 0.004960326734452432, 207: 0.0012878724331073668, 208: 8.99835639040803, 209: 0.8996912741131945, 210: 9.099182108918027, 211: 9.047239144971902, 212: 5.6376837780179e-05, 213: 9.205656890462903, 214: 0.008592156623310698, 215: 0.9900357758425912, 216: 0.9002177696262985, 217: 0.0015685106088179285, 218: 0.0043098592890551774, 219: 0.00343764419847989, 220: 0.004944962346831754, 221: 0.013024574248697789, 223: 0.00923838973411376, 224: 0.004525942796826309, 225: 0.004958588381561725, 226: 0.00020000000000000573, 227: 1.886756853644063e-05, 228: 0.0004017751469565537, 229: 10.0, 230: 0.011254134905796227, 231: 0.0, 232: 3.3898190174644294e-06, 233: 0.0, 235: 4.871794871796897e-05, 236: 2.3333, 237: 0.001203620964571028, 238: 0.0, 239: 0.00032307568047811643, 240: 3.636363636361217e-05, 242: 9.140759373864446, 243: 0.019426202637395244, 244: 9.0, 245: 0.0, 246: 0.0, 247: 10.0, 249: 8.95107388672361, 250: 8.999920000639994, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.984375, 260: 0.0, 261: 0.0, 262: 0.9012345679012346, 263: 0.0, 264: 0.0, 265: 0.9047401310775797, 266: 0.0, 267: 0.0, 268: 0.984375, 269: 0.9027777777777778, 270: 0.0, 271: 0.9012345679012346, 272: 0.9012345679012346, 273: 0.0, 274: 0.0, 275: 0.9027777777777778, 276: 10, 277: 0.781876559582599, 278: 10.0, 280: 0.9702119127053536, 281: 0.3595481796445272, 282: 0.08063730222209968, 283: 0.980883140742556, 284: 0.0034000000000000696, 285: 0.8691182191819513, 286: 10, 287: 0.442584036285024, 288: 10, 289: 0.9523065839243066, 290: 0.9243842237319355, 291: 0.682492447317347, 292: 0.029377507441439177, 293: 0.942966918308476, 294: 0.1249220385965442, 295: 0.9720632498198313, 296: 10, 297: 0.9815582197780717, 298: 0.9872093866965816, 299: 0.44311410591969713, 300: 0.9951718522492735, 301: 0.6321230180627598, 304: 10, 305: 0.8940544037789292, 306: 0.0, 307: 2.9493423457881523e-05, 309: 0.8646636892678305, 310: 0.6321230180627598, 311: 10, 312: 10, 313: 0.4621197859236748, 315: 0.0, 316: 10, 317: 0.00012481408507916938, 318: 0.0, 319: 10, 321: 0.0, 322: 10, 323: 10, 325: 10, 327: 10, 328: 0.01694915254237288, 329: 8.843903810997046, 330: 10.0, 331: 10.0, 332: 0.0, 333: 0.1646090534979424, 334: 10, 335: 10.0, 336: 2.5, 337: 10, 338: 0.0015117157974301964, 339: 0.3333333333333333, 340: 10, 341: 0.26209195453499345, 342: 0.9078748107016659, 343: 10, 344: 10.0, 345: 0.9032882011605415, 346: 1.7669115542410077, 347: 1.0002258723188955, 348: 10.0, 349: 0.4166666666666667, 350: 0.00773333333333337, 351: 0.0, 352: 0.4074, 353: 0.29290000000000005, 354: 0.04290000000000005, 355: 1.2071, 356: 1.7071, 357: 1.9641475665377288, 358: 1.7071, 359: 0.0, 360: 0.0, 362: 1.0, 363: 2.0, 364: 0.0, 365: 0.5, 366: 1.5, 367: 0.0, 368: 1.0, 369: 0.4226661278217193, 370: 1.5, 371: 0.29290000000000005, 372: 0.134, 373: 1.1625999999999999, 375: 1.7071, 376: 1.0634202053261295, 377: 1.5346991574310387, 378: 2.5019345340028067, 379: 0.6909117353723404, 380: 10.0, 381: 0.38397926173490154, 382: 10.0, 384: 10.0, 385: 0.8370073480293923, 386: 10.0, 387: 0.6609916119923596, 388: 10.0, 389: 0.5854621578767372, 390: 10.0, 391: 0.7359595671663098, 392: 0.3430548951233687, 393: 1.7907616167170741, 394: 1.7146508254472612, 395: 0.6604141276418979, 396: 1.3168218321370193, 397: 1.2360476547126038, 398: 0.1011350750541715, 399: 1.7468550749612268, 400: 1.4862255263342417}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 2.0, 18: 1.0, 19: 0.0, 20: 0.0, 21: 10, 22: 0.0, 23: 0.0, 24: 2.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.11235955056179775, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 2.0, 42: 0.0, 43: 2.1451612903225805, 44: 0.0, 45: 2.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 2.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.39457459926017263, 65: 2.0, 66: 0.0, 67: 0.0, 68: 0.030534351145038167, 69: 0.06354916067146282, 70: 0.011111111111111112, 71: 0.0, 72: 0.0, 73: 2.0408163265306123, 74: 0.25125628140703515, 75: 0.0, 76: 0.999998998676325, 77: 0.02153187663163325, 78: 0.037101445219012985, 79: 0.3805124972361365, 80: 8.880656074963407e-07, 81: 0.010091379192163377, 82: 9.022857573128268e-08, 83: 0.8370729758925709, 84: 5.265504730000651e-08, 85: 8.574319808160072e-07, 86: 6.468847827153158e-06, 87: 0.32084993258895805, 88: 0.4501898090856154, 89: 10, 90: 10, 91: 10, 92: 10, 93: 10, 94: 10, 95: 10, 96: 10, 97: 10, 98: 10, 99: 10, 100: 10, 101: 0.0, 102: 0.0, 103: 1.5, 104: 1.0, 105: 1.75, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 10.0, 114: 0.6153846153846154, 115: 0.8, 116: 0.0, 117: 2.0, 118: 1.25, 119: 1.0909090909090908, 120: 0.0, 121: 0.9333333333333333, 122: 0.2222222222222222, 123: 2.0, 124: 0.9090909090909091, 125: 0.36363636363636365, 126: 0.0, 127: 0.006900000000000017, 128: 1.9989761965702586, 129: 0.0004043818637006199, 130: 0.007400000000000018, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.001920347332387049, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 2.0, 140: 0.0010000000000000009, 141: 0.3, 142: 2.0, 143: 1.6710526315789473, 144: 0.02, 145: 0.37999999999999995, 146: 0.625, 147: 0.0, 148: 0.0004852353391394181, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.018018018018018018, 154: 0.0, 155: 8.181818181818182, 156: 0.07177033492822966, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.018674136321195144, 161: 0.016722408026755852, 162: 0.020050125313283207, 163: 0.004553734061930784, 164: 0.02145002145002145, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.006064281382656155, 169: 0.014892032762472078, 170: 0.002932551319648094, 171: 0.0, 172: 0.0, 173: 0.012077294685990338, 174: 0.026954177897574125, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 8.1, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 10, 188: 10, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 9.001436454429912, 202: 0.000408557836845193, 204: 0.8986934250700569, 205: 0.9000933928425443, 206: 0.004960326734452432, 207: 0.0012878724331073668, 208: 8.99835639040803, 209: 0.8996912741131945, 210: 9.099182108918027, 211: 9.047239144971902, 212: 5.6376837780179e-05, 213: 9.205656890462903, 214: 0.008592156623310698, 215: 0.9900357758425912, 216: 0.9002177696262985, 217: 0.0015685106088179285, 218: 0.0043098592890551774, 219: 0.00343764419847989, 220: 0.004944962346831754, 221: 0.013024574248697789, 223: 0.00923838973411376, 224: 0.004525942796826309, 225: 0.004958588381561725, 226: 0.0, 227: 0.0, 228: 0.0, 229: 10.0, 230: 0.011254134905796227, 231: 0.0, 232: 0.0, 233: 0.0, 235: 0.0, 236: 2.3333, 237: 0.001203620964571028, 238: 0.0, 239: 0.0, 240: 0.0, 242: 9.140759373864446, 243: 0.019426202637395244, 244: 9.0, 245: 0.0, 246: 0.0, 247: 10.0, 249: 8.95107388672361, 250: 8.999920000639994, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.984375, 260: 0.0, 261: 0.0, 262: 0.9012345679012346, 263: 0.0, 264: 0.0, 265: 0.9047401310775797, 266: 0.0, 267: 0.0, 268: 0.984375, 269: 0.9027777777777778, 270: 0.0, 271: 0.9012345679012346, 272: 0.9012345679012346, 273: 0.0, 274: 0.0, 275: 0.9027777777777778, 276: 10, 277: 0.781876559582599, 278: 10.0, 280: 0.9702119127053536, 281: 0.3595481796445272, 282: 0.08063730222209968, 283: 0.980883140742556, 284: 0.0034000000000000696, 285: 0.8691182191819513, 286: 10, 287: 0.442584036285024, 288: 10, 289: 0.9523065839243066, 290: 0.9243842237319355, 291: 0.682492447317347, 292: 0.029377507441439177, 293: 0.942966918308476, 294: 0.1249220385965442, 295: 0.9720632498198313, 296: 10, 297: 0.9815582197780717, 298: 0.9872093866965816, 299: 0.44311410591969713, 300: 0.9951718522492735, 301: 0.6321230180627598, 304: 10, 305: 0.8940544037789292, 306: 0.0, 307: 0.0, 309: 0.8646636892678305, 310: 0.6321230180627598, 311: 10, 312: 10, 313: 0.4621197859236748, 315: 0.0, 316: 10, 317: 0.00012481408507916938, 318: 0.0, 319: 10, 321: 0.0, 322: 10, 323: 10, 325: 10, 327: 10, 328: 0.01694915254237288, 329: 8.843903810997046, 330: 10.0, 331: 10.0, 332: 0.0, 333: 0.1646090534979424, 334: 10, 335: 10.0, 336: 2.5, 337: 10, 338: 0.0015117157974301964, 339: 0.3333333333333333, 340: 10, 341: 0.26209195453499345, 342: 0.9078748107016659, 343: 10, 344: 10.0, 345: 0.9032882011605415, 346: 1.7669115542410077, 347: 1.0002258723188955, 348: 10.0, 349: 0.4166666666666667, 350: 0.00773333333333337, 351: 0.0, 352: 0.4074, 353: 0.29290000000000005, 354: 0.04290000000000005, 355: 1.2071, 356: 1.7071, 357: 1.9641475665377288, 358: 1.7071, 359: 0.0, 360: 0.0, 362: 1.0, 363: 2.0, 364: 0.0, 365: 0.5, 366: 1.5, 367: 0.0, 368: 1.0, 369: 0.4226661278217193, 370: 1.5, 371: 0.29290000000000005, 372: 0.134, 373: 1.1625999999999999, 375: 1.7071, 376: 1.0634202053261295, 377: 1.5346991574310387, 378: 2.5019345340028067, 379: 0.6909117353723404, 380: 10.0, 381: 0.38397926173490154, 382: 10.0, 384: 10.0, 385: 0.8370073480293923, 386: 10.0, 387: 0.6609916119923596, 388: 10.0, 389: 0.5854621578767372, 390: 10.0, 391: 0.7359595671663098, 392: 0.3430548951233687, 393: 1.7907616167170741, 394: 1.7146508254472612, 395: 0.6604141276418979, 396: 1.3168218321370193, 397: 1.2360476547126038, 398: 0.1011350750541715, 399: 1.7468550749612268, 400: 1.4862255263342417}</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.12658227848101267, 41: 0.5882352941176471, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0012970168612191958, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 1.743664368566302e-10, 77: 2.068163434780804e-05, 78: 0.03339130386873335, 79: 0.0002463293111841728, 80: 0.010106323016466868, 81: 0.0, 82: 0.1652802885849833, 83: 0.6293687982683304, 84: 0.9000000000283106, 85: 0.0, 86: 6.915669215143585e-06, 87: 7.211731458506587e-07, 88: 0.0, 89: 3.4043255615398694e-10, 90: 3.6339005007031206e-05, 91: 0.999989992754191, 92: 1.9671491699198727e-07, 93: 0.9999900000037081, 94: 0.0013310279430704427, 95: 0.2558510754722497, 96: 0.0, 97: 3.291497429477172e-05, 98: 1.1953887114378692e-07, 99: 0.0, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0008087637274012398, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0010000000000000009, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.02, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.028673835125448053, 150: 0.0, 151: 0.019230769230769232, 152: 0.007680491551459293, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.004668534080298786, 161: 0.027870680044593088, 162: 0.0, 163: 0.0, 164: 0.02145002145002145, 165: 0.0055617352614015575, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.007446016381236039, 170: 0.0, 171: 0.020202020202020204, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 10.0, 202: 0.0006518862940404747, 203: 0.0015022449563514703, 204: 0.016826661651428335, 205: 0.023335260337728713, 206: 0.00023422755284661782, 207: 0.900157639380066, 208: 0.006882192054452593, 209: 0.0007461016138337949, 210: 0.98997747998939, 211: 0.900579894382024, 212: 0.8997369287389145, 213: 0.0014426032520880666, 214: 0.8899305776162655, 215: 0.9006635854209994, 216: 0.9010399283769647, 217: 0.9007538131550479, 218: 0.010531821548960131, 219: 0.0339588053441443, 220: 8.900266597095968, 221: 0.0005573767841682046, 222: 10.0, 223: 0.9008595178685088, 224: 0.9898462173620903, 225: 9.18402914470025, 226: 0.019199999999999995, 227: 0.0, 228: 0.12854030501089322, 229: 1.5789999999960003e-05, 230: 0.012377750611246938, 231: 0.0, 232: 0.0010203355242862987, 233: 0.0, 234: 0.0, 235: 10.0, 236: 3.333333333332966e-05, 237: 0.0035978034463170095, 238: 0.0, 239: 3.846135207069057e-06, 240: 0.0006370370370369915, 241: 0.001084828944442655, 242: 0.07043039072909245, 243: 0.2597527574209786, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0005928686372492123, 248: 10.0, 249: 0.17074384277303256, 250: 7.999936000404534e-06, 251: 0.0, 252: 0.6666666666666666, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.8571428571428571, 258: 0.0, 259: 10.0, 260: 0.8571428571428571, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.6666666666666666, 268: 10.0, 269: 0.0, 270: 0.6666666666666666, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.903226790839957, 277: 0.9920720854345891, 278: 0.8365716023989797, 279: 0.7457189806980109, 280: 0.9686694954598949, 281: 0.5523357456668019, 282: 10, 283: 0.8654341281040824, 284: 0.0040999999999999925, 285: 10.0, 286: 0.33295012670922286, 287: 10.0, 288: 0.9775171179605652, 289: 0.3106663169132673, 290: 0.9819981658328425, 291: 0.9880303026985284, 292: 10, 293: 10.0, 294: 0.09609967007637965, 295: 10.0, 296: 10.0, 298: 0.9859483265353375, 299: 0.05186994327719387, 300: 0.9934998959889124, 301: 0.6321230180627598, 302: 0.40461128559308157, 303: 0.46387419365848664, 304: 0.5146638392941667, 305: 0.0035005834305717747, 306: 0.0, 307: 0.0004774789113481002, 308: 6.079643327595279e-05, 309: 0.51278928136419, 310: 0.6321230180627598, 311: 10, 312: 0.0, 313: 0.7310598929618374, 314: 2.141592653589793, 315: 0.0, 316: 10, 317: 0.00043154998749457964, 318: 0.0, 319: 10, 320: 0.0, 321: 0.0, 322: 1.0, 323: 1.1913485559013017, 324: 0.46387419365848664, 325: 10, 326: 10.0, 327: 0.016544117647058824, 328: 0.0, 329: 0.06248535133361467, 330: 0.8632, 331: 10.0, 332: 0.0, 333: 0.0, 334: 0.023460371725732003, 335: 10.0, 336: 0.0, 337: 0.8393625907601362, 338: 0.005418304358780586, 339: 0.0, 340: 0.06574600368941069, 341: 0.0, 342: 0.0, 343: 0.09288824383164002, 344: 0.0014571174745129107, 345: 0.8549323017408124, 346: 10.0, 347: 1.0, 348: 0.00030000000000002247, 349: 0.0, 350: 0.00773333333333337, 351: 0.5, 352: 0.4226, 353: 1.2071, 354: 1.4142067811999999, 355: 0.29290000000000005, 356: 1.7071, 357: 2.732001616534842, 358: 6.7812000000833095e-06, 359: 0.5, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 2.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 0.0, 368: 1.0, 369: 0.4226661278217193, 370: 1.5, 371: 0.20709999999999995, 372: 0.134, 373: 0.5594, 374: 0.29290000000000005, 375: 1.7071, 376: 0.5415578112439925, 377: 0.04884103066111944, 378: 0.6673150669704886, 379: 0.7314937943262412, 380: 0.6368621352866554, 381: 0.0711913790517814, 382: 1.8443249253364706, 383: 0.19896888675738872, 384: 0.15985879979828543, 385: 0.8370073480293923, 386: 2.013502553319315, 387: 0.6609916119923596, 388: 0.1422175010565513, 389: 0.6890966184075529, 390: 0.3771757902703124, 391: 0.3194644630216842, 392: 0.19708143477738674, 393: 0.07403079461094302, 394: 0.10865510810250742, 395: 2.7454398054316984, 396: 0.5990334731007035, 397: 0.28779903437760906, 398: 0.12272507831007418, 399: 0.3779079786317423, 400: 0.44066428737961577}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.12658227848101267, 41: 0.5882352941176471, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0012970168612191958, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 1.743664368566302e-10, 77: 2.068163434780804e-05, 78: 0.03339130386873335, 79: 0.0002463293111841728, 80: 0.010106323016466868, 81: 0.0, 82: 0.1652802885849833, 83: 0.6293687982683304, 84: 0.9000000000283106, 85: 0.0, 86: 6.915669215143585e-06, 87: 7.211731458506587e-07, 88: 0.0, 89: 3.4043255615398694e-10, 90: 3.6339005007031206e-05, 91: 0.999989992754191, 92: 1.9671491699198727e-07, 93: 0.9999900000037081, 94: 0.0013310279430704427, 95: 0.2558510754722497, 96: 0.0, 97: 3.291497429477172e-05, 98: 1.1953887114378692e-07, 99: 0.0, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0008087637274012398, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0010000000000000009, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.02, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.028673835125448053, 150: 0.0, 151: 0.019230769230769232, 152: 0.007680491551459293, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.004668534080298786, 161: 0.027870680044593088, 162: 0.0, 163: 0.0, 164: 0.02145002145002145, 165: 0.0055617352614015575, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.007446016381236039, 170: 0.0, 171: 0.020202020202020204, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 10.0, 202: 0.0006518862940404747, 203: 0.0015022449563514703, 204: 0.016826661651428335, 205: 0.023335260337728713, 206: 0.00023422755284661782, 207: 0.900157639380066, 208: 0.006882192054452593, 209: 0.0007461016138337949, 210: 0.98997747998939, 211: 0.900579894382024, 212: 0.8997369287389145, 213: 0.0014426032520880666, 214: 0.8899305776162655, 215: 0.9006635854209994, 216: 0.9010399283769647, 217: 0.9007538131550479, 218: 0.010531821548960131, 219: 0.0339588053441443, 220: 8.900266597095968, 221: 0.0005573767841682046, 222: 10.0, 223: 0.9008595178685088, 224: 0.9898462173620903, 225: 9.18402914470025, 226: 0.019199999999999995, 227: 0.0, 228: 0.12854030501089322, 229: 0.0, 230: 0.012377750611246938, 231: 0.0, 232: 0.0010203355242862987, 233: 0.0, 234: 0.0, 235: 10.0, 236: 0.0, 237: 0.0035978034463170095, 238: 0.0, 239: 0.0, 240: 0.0, 241: 0.001084828944442655, 242: 0.07043039072909245, 243: 0.2597527574209786, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 10.0, 249: 0.17074384277303256, 250: 0.0, 251: 0.0, 252: 0.6666666666666666, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.8571428571428571, 258: 0.0, 259: 10.0, 260: 0.8571428571428571, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.6666666666666666, 268: 10.0, 269: 0.0, 270: 0.6666666666666666, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.903226790839957, 277: 0.9920720854345891, 278: 0.8365716023989797, 279: 0.7457189806980109, 280: 0.9686694954598949, 281: 0.5523357456668019, 282: 10, 283: 0.8654341281040824, 284: 0.0040999999999999925, 285: 10.0, 286: 0.33295012670922286, 287: 10.0, 288: 0.9775171179605652, 289: 0.3106663169132673, 290: 0.9819981658328425, 291: 0.9880303026985284, 292: 10, 293: 10.0, 294: 0.09609967007637965, 295: 10.0, 296: 10.0, 298: 0.9859483265353375, 299: 0.05186994327719387, 300: 0.9934998959889124, 301: 0.6321230180627598, 302: 0.40461128559308157, 303: 0.46387419365848664, 304: 0.5146638392941667, 305: 0.0035005834305717747, 306: 0.0, 307: 0.0004774789113481002, 308: 0.0, 309: 0.51278928136419, 310: 0.6321230180627598, 311: 10, 312: 0.0, 313: 0.7310598929618374, 314: 2.141592653589793, 315: 0.0, 316: 10, 317: 0.00043154998749457964, 318: 0.0, 319: 10, 320: 0.0, 321: 0.0, 322: 1.0, 323: 1.1913485559013017, 324: 0.46387419365848664, 325: 10, 326: 10.0, 327: 0.016544117647058824, 328: 0.0, 329: 0.06248535133361467, 330: 0.8632, 331: 10.0, 332: 0.0, 333: 0.0, 334: 0.023460371725732003, 335: 10.0, 336: 0.0, 337: 0.8393625907601362, 338: 0.005418304358780586, 339: 0.0, 340: 0.06574600368941069, 341: 0.0, 342: 0.0, 343: 0.09288824383164002, 344: 0.0014571174745129107, 345: 0.8549323017408124, 346: 10.0, 347: 1.0, 348: 0.0, 349: 0.0, 350: 0.00773333333333337, 351: 0.5, 352: 0.4226, 353: 1.2071, 354: 1.4142067811999999, 355: 0.29290000000000005, 356: 1.7071, 357: 2.732001616534842, 358: 0.0, 359: 0.5, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 2.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 0.0, 368: 1.0, 369: 0.4226661278217193, 370: 1.5, 371: 0.20709999999999995, 372: 0.134, 373: 0.5594, 374: 0.29290000000000005, 375: 1.7071, 376: 0.5415578112439925, 377: 0.04884103066111944, 378: 0.6673150669704886, 379: 0.7314937943262412, 380: 0.6368621352866554, 381: 0.0711913790517814, 382: 1.8443249253364706, 383: 0.19896888675738872, 384: 0.15985879979828543, 385: 0.8370073480293923, 386: 2.013502553319315, 387: 0.6609916119923596, 388: 0.1422175010565513, 389: 0.6890966184075529, 390: 0.3771757902703124, 391: 0.3194644630216842, 392: 0.19708143477738674, 393: 0.07403079461094302, 394: 0.10865510810250742, 395: 2.7454398054316984, 396: 0.5990334731007035, 397: 0.28779903437760906, 398: 0.12272507831007418, 399: 0.3779079786317423, 400: 0.44066428737961577}</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 2.0, 16: 0.0, 17: 1.6666666666666667, 18: 1.3333333333333333, 19: 0.1, 20: 0.0, 21: 1.0, 22: 0.0, 23: 0.0, 24: 3.0, 25: 0.0, 26: 0.3401360544217687, 27: 0.0, 28: 0.0125, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.11235955056179775, 37: 0.0, 38: 0.0, 39: 0.4, 40: 0.12658227848101267, 41: 5.176470588235294, 42: 0.0, 43: 1.032258064516129, 44: 0.0, 45: 1.5, 46: 0.5263157894736842, 47: 0.5882352941176471, 48: 0.0, 49: 3.4, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.7878787878787878, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.07936507936507936, 66: 0.12224938875305623, 67: 0.24154589371980675, 68: 0.3053435114503817, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.3401360544217687, 74: 0.0, 75: 0.0, 76: 3.487328737132604e-10, 77: 1.0344437727108508e-09, 78: 0.14193241159702324, 79: 4.926684757378604e-08, 80: 0.0, 81: 0.0, 82: 0.0, 83: 0.629369030739085, 84: 0.0, 85: 0.0, 86: 6.915669215143584e-05, 87: 0.0, 88: 2.7423905108620024e-06, 89: 1.1347751871799565e-07, 90: 3.659517120546949e-11, 91: 7.603221286567108e-09, 92: 0.0, 93: 0.0042106732875802425, 94: 0.0, 95: 1.1000000255339675, 96: 0.0, 97: 0.0, 98: 6.123917579087443e-08, 99: 1.3471512710905443e-08, 100: 9.328129583895493e-06, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 10.0, 114: 0.0, 115: 0.0, 116: 1.3333333333333333, 117: 0.0, 118: 0.0, 119: 0.0, 120: 4.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.013800000000000034, 128: 0.0, 129: 0.0008087637274012398, 130: 0.0, 131: 0.00020000000000000226, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.06332119677061897, 137: 0.0, 138: 0.19799999999999995, 139: 2.0, 140: 0.0010000000000000009, 141: 0.3, 142: 2.0, 143: 0.0, 144: 0.0, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0004852353391394181, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.023923444976076555, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.05042016806722689, 161: 0.029542920847268672, 162: 0.0, 163: 0.006830601092896175, 164: 0.00858000858000858, 165: 0.03337041156840934, 166: 0.0, 167: 0.0, 168: 0.01212856276531231, 169: 0.029784065524944156, 170: 0.0, 171: 0.0, 172: 0.08760951188986232, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.405, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 4.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.029320950174234656, 202: 0.9000399316735939, 203: 0.9900778780677968, 204: 1.0, 205: 0.9005572136646651, 206: 0.9000935914787567, 207: 0.9900310099320591, 208: 0.9008387285479071, 209: 10, 210: 8.82358738678542, 211: 0.9896329566157136, 212: 0.8999789014607162, 213: 0.903526378085072, 214: 0.05889515381726157, 215: 0.8972766935464156, 216: 0.9041161705747836, 217: 0.9899427020414572, 218: 0.8993908923779054, 219: 0.901333901983104, 220: 0.9900421910109578, 221: 0.8972220882778619, 222: 0.9015996015687234, 223: 0.9901128612525255, 224: 0.9930981593351993, 225: 0.9905370426374366, 226: 0.002439836221791475, 227: 10.0, 228: 0.12854030501089322, 229: 8.473700000000001, 230: 9.31479217603912, 231: 8.23076923076923, 232: 0.05085067508245728, 233: 0.0, 234: 4.545454545457073e-05, 235: 10.0, 236: 3.333333333332966e-05, 237: 0.09614656315091841, 238: 0.0, 239: 0.19231079880461996, 240: 0.006399999999999961, 241: 4.717734506527747, 242: 0.01419192169581035, 243: 10.0, 244: 0.0, 245: 0.8095238095238095, 246: 0.0, 247: 0.05869399508765979, 248: 0.0015000000000000013, 249: 0.17074384277303256, 250: 5.479948160414716, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 5.823823406913786, 258: 0.0, 259: 0.9375, 260: 5.823823406913786, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.5378753238835543, 266: 0.0, 267: 0.0, 268: 0.9375, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8767706308661635, 277: 0.9185653585076866, 278: 0.999992217828248, 279: 0.9955863057905967, 280: 0.9727336106599541, 281: 0.9258531365102548, 282: 0.8387162019288229, 283: 0.9739463599413027, 284: 0.03317777777777775, 285: 0.947358830427046, 286: 0.9634580514265007, 287: 0.383302954516553, 288: 0.9143223528958552, 289: 0.9663622222303749, 290: 0.9739592533646291, 291: 0.8782760833054145, 292: 0.13213407532030552, 293: 0.5106634751120114, 294: 0.04247728950421079, 295: 0.9532222792330148, 296: 0.9996907341285218, 297: 0.98347847014368, 298: 0.9584574469192972, 299: 0.944313178466018, 300: 0.9950400148658203, 301: 0.6321230180627598, 302: 0.255764106991352, 303: 0.12283695689272675, 304: 0.8933297991177084, 305: 1.0, 306: 0.0, 307: 0.36336145153589056, 308: 0.020822789239031376, 309: 0.8646636892678305, 310: 0.8393849096862008, 311: 1.0, 312: 1.0, 313: 0.19317967888551224, 314: 0.0, 315: 0.0, 316: 10, 317: 0.0004774789113481002, 318: 0.0, 319: 10, 320: 0.0, 321: 0.0, 322: 1.0, 323: 3.191348555901302, 324: 0.12283695689272675, 325: 10, 326: 0.9398137962490944, 327: 0.9227941176470589, 328: 0.0, 329: 0.406271972999578, 330: 0.8632, 331: 0.3447, 332: 0.0, 333: 0.20164609053497942, 334: 0.7592449922958397, 335: 0.5778, 336: 0.0, 337: 10, 338: 10.0, 339: 0.3466666666666667, 340: 0.7582267907636904, 341: 0.006524407981010599, 342: 0.08892815076560659, 343: 1.7982583454281569, 344: 1.4055809477988934, 345: 0.0, 346: 0.9045892567503101, 347: 1.0, 348: 6.6863, 349: 0.0, 350: 10.0, 351: 0.0, 352: 0.4226, 353: 0.9071, 354: 1.2071, 355: 1.57312, 356: 1.4142067811999999, 357: 10, 358: 1.0821, 359: 0.0, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 2.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 1.0, 368: 0.0, 369: 0.4226661278217193, 370: 1.5, 371: 6.7812000000833095e-06, 372: 2.5403800000045607e-05, 373: 10, 374: 5.8550778260000005, 375: 1.7071, 376: 0.43181428121307014, 377: 0.11484676231863433, 378: 0.7156255115878397, 379: 0.04308387693426024, 380: 0.6930883496337521, 381: 0.03592775885339674, 382: 0.3910952690045858, 383: 0.5503866674659792, 384: 0.7589792532129158, 385: 0.00263489942848656, 386: 0.6434696605587263, 387: 0.6609916119923596, 388: 0.1422175010565513, 389: 0.06743494346740184, 390: 0.6642927832650922, 391: 0.1827613086380077, 392: 0.07661013367147458, 393: 0.031069562826505297, 394: 0.06992470815776744, 395: 0.7750735318009365, 396: 0.0695318554764119, 397: 0.34050861498483453, 398: 0.10181993735194066, 399: 0.09529553679131483, 400: 0.2535655114686885}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 2.0, 16: 0.0, 17: 1.6666666666666667, 18: 1.3333333333333333, 19: 0.1, 20: 0.0, 21: 1.0, 22: 0.0, 23: 0.0, 24: 3.0, 25: 0.0, 26: 0.3401360544217687, 27: 0.0, 28: 0.0125, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.11235955056179775, 37: 0.0, 38: 0.0, 39: 0.4, 40: 0.12658227848101267, 41: 5.176470588235294, 42: 0.0, 43: 1.032258064516129, 44: 0.0, 45: 1.5, 46: 0.5263157894736842, 47: 0.5882352941176471, 48: 0.0, 49: 3.4, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.7878787878787878, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.07936507936507936, 66: 0.12224938875305623, 67: 0.24154589371980675, 68: 0.3053435114503817, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.3401360544217687, 74: 0.0, 75: 0.0, 76: 3.487328737132604e-10, 77: 1.0344437727108508e-09, 78: 0.14193241159702324, 79: 4.926684757378604e-08, 80: 0.0, 81: 0.0, 82: 0.0, 83: 0.629369030739085, 84: 0.0, 85: 0.0, 86: 6.915669215143584e-05, 87: 0.0, 88: 2.7423905108620024e-06, 89: 1.1347751871799565e-07, 90: 3.659517120546949e-11, 91: 7.603221286567108e-09, 92: 0.0, 93: 0.0042106732875802425, 94: 0.0, 95: 1.1000000255339675, 96: 0.0, 97: 0.0, 98: 6.123917579087443e-08, 99: 1.3471512710905443e-08, 100: 9.328129583895493e-06, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 10.0, 114: 0.0, 115: 0.0, 116: 1.3333333333333333, 117: 0.0, 118: 0.0, 119: 0.0, 120: 4.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.013800000000000034, 128: 0.0, 129: 0.0008087637274012398, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.06332119677061897, 137: 0.0, 138: 0.19799999999999995, 139: 2.0, 140: 0.0010000000000000009, 141: 0.3, 142: 2.0, 143: 0.0, 144: 0.0, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0004852353391394181, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.023923444976076555, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.05042016806722689, 161: 0.029542920847268672, 162: 0.0, 163: 0.006830601092896175, 164: 0.00858000858000858, 165: 0.03337041156840934, 166: 0.0, 167: 0.0, 168: 0.01212856276531231, 169: 0.029784065524944156, 170: 0.0, 171: 0.0, 172: 0.08760951188986232, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.405, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 4.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.029320950174234656, 202: 0.9000399316735939, 203: 0.9900778780677968, 204: 1.0, 205: 0.9005572136646651, 206: 0.9000935914787567, 207: 0.9900310099320591, 208: 0.9008387285479071, 209: 10, 210: 8.82358738678542, 211: 0.9896329566157136, 212: 0.8999789014607162, 213: 0.903526378085072, 214: 0.05889515381726157, 215: 0.8972766935464156, 216: 0.9041161705747836, 217: 0.9899427020414572, 218: 0.8993908923779054, 219: 0.901333901983104, 220: 0.9900421910109578, 221: 0.8972220882778619, 222: 0.9015996015687234, 223: 0.9901128612525255, 224: 0.9930981593351993, 225: 0.9905370426374366, 226: 0.002439836221791475, 227: 10.0, 228: 0.12854030501089322, 229: 8.473700000000001, 230: 9.31479217603912, 231: 8.23076923076923, 232: 0.05085067508245728, 233: 0.0, 234: 0.0, 235: 10.0, 236: 0.0, 237: 0.09614656315091841, 238: 0.0, 239: 0.19231079880461996, 240: 0.006399999999999961, 241: 4.717734506527747, 242: 0.01419192169581035, 243: 10.0, 244: 0.0, 245: 0.8095238095238095, 246: 0.0, 247: 0.05869399508765979, 248: 0.0015000000000000013, 249: 0.17074384277303256, 250: 5.479948160414716, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 5.823823406913786, 258: 0.0, 259: 0.9375, 260: 5.823823406913786, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.5378753238835543, 266: 0.0, 267: 0.0, 268: 0.9375, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8767706308661635, 277: 0.9185653585076866, 278: 0.999992217828248, 279: 0.9955863057905967, 280: 0.9727336106599541, 281: 0.9258531365102548, 282: 0.8387162019288229, 283: 0.9739463599413027, 284: 0.03317777777777775, 285: 0.947358830427046, 286: 0.9634580514265007, 287: 0.383302954516553, 288: 0.9143223528958552, 289: 0.9663622222303749, 290: 0.9739592533646291, 291: 0.8782760833054145, 292: 0.13213407532030552, 293: 0.5106634751120114, 294: 0.04247728950421079, 295: 0.9532222792330148, 296: 0.9996907341285218, 297: 0.98347847014368, 298: 0.9584574469192972, 299: 0.944313178466018, 300: 0.9950400148658203, 301: 0.6321230180627598, 302: 0.255764106991352, 303: 0.12283695689272675, 304: 0.8933297991177084, 305: 1.0, 306: 0.0, 307: 0.36336145153589056, 308: 0.020822789239031376, 309: 0.8646636892678305, 310: 0.8393849096862008, 311: 1.0, 312: 1.0, 313: 0.19317967888551224, 314: 0.0, 315: 0.0, 316: 10, 317: 0.0004774789113481002, 318: 0.0, 319: 10, 320: 0.0, 321: 0.0, 322: 1.0, 323: 3.191348555901302, 324: 0.12283695689272675, 325: 10, 326: 0.9398137962490944, 327: 0.9227941176470589, 328: 0.0, 329: 0.406271972999578, 330: 0.8632, 331: 0.3447, 332: 0.0, 333: 0.20164609053497942, 334: 0.7592449922958397, 335: 0.5778, 336: 0.0, 337: 10, 338: 10.0, 339: 0.3466666666666667, 340: 0.7582267907636904, 341: 0.006524407981010599, 342: 0.08892815076560659, 343: 1.7982583454281569, 344: 1.4055809477988934, 345: 0.0, 346: 0.9045892567503101, 347: 1.0, 348: 6.6863, 349: 0.0, 350: 10.0, 351: 0.0, 352: 0.4226, 353: 0.9071, 354: 1.2071, 355: 1.57312, 356: 1.4142067811999999, 357: 10, 358: 1.0821, 359: 0.0, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 2.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 1.0, 368: 0.0, 369: 0.4226661278217193, 370: 1.5, 371: 0.0, 372: 0.0, 373: 10, 374: 5.8550778260000005, 375: 1.7071, 376: 0.43181428121307014, 377: 0.11484676231863433, 378: 0.7156255115878397, 379: 0.04308387693426024, 380: 0.6930883496337521, 381: 0.03592775885339674, 382: 0.3910952690045858, 383: 0.5503866674659792, 384: 0.7589792532129158, 385: 0.00263489942848656, 386: 0.6434696605587263, 387: 0.6609916119923596, 388: 0.1422175010565513, 389: 0.06743494346740184, 390: 0.6642927832650922, 391: 0.1827613086380077, 392: 0.07661013367147458, 393: 0.031069562826505297, 394: 0.06992470815776744, 395: 0.7750735318009365, 396: 0.0695318554764119, 397: 0.34050861498483453, 398: 0.10181993735194066, 399: 0.09529553679131483, 400: 0.2535655114686885}</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 10, 16: 0.125, 17: 0.0, 18: 10, 19: 10, 20: 0.0, 21: 2.0, 22: 0.0, 23: 0.3333333333333333, 24: 6.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.125, 30: 0.0, 31: 0.16129032258064516, 32: 0.4588235294117647, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.11235955056179775, 37: 0.21333333333333335, 38: 0.0, 39: 0.0, 40: 0.0, 41: 2.1176470588235294, 42: 10, 43: 1.3548387096774193, 44: 0.0, 45: 1.7857142857142858, 46: 10, 47: 10, 48: 10, 49: 1.6, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.19083969465648856, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.3801478352692714, 63: 0.5336481700118064, 64: 2.0, 65: 2.1507936507936507, 66: 0.1295843520782396, 67: 0.0, 68: 0.06870229007633588, 69: 2.6906474820143886, 70: 0.0, 71: 0.020440251572327043, 72: 0.0, 73: 10, 74: 2.0, 75: 7.946666666666666, 76: 0.3854096986644142, 77: 10, 78: 10, 79: 0.5772101972188735, 80: 0.9467914187910013, 81: 0.8989301591490884, 82: 0.9999183637573495, 83: 0.9999990699300358, 84: 0.5377674225061444, 85: 10.0, 86: 0.3358422451203626, 87: 0.6435213709489571, 88: 0.0017165279187326167, 89: 1.0, 90: 10.0, 91: 10, 92: 2.2677298971756623, 93: 0.9999999044979762, 94: 1.0079559050507094, 95: 10.0, 96: 1.0014427149799703, 97: 0.9999999999700772, 98: 0.5075955023281672, 99: 0.7348516181958211, 100: 10, 101: 0.0, 102: 0.8571428571428571, 103: 1.0, 104: 1.0, 105: 0.125, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.2857142857142857, 111: 0.0, 112: 0.0, 113: 10.0, 114: 0.0, 115: 0.0, 116: 10, 117: 10, 118: 1.625, 119: 0.0, 120: 10, 121: 0.0, 122: 1.7777777777777777, 123: 1.75, 124: 0.0, 125: 0.0, 126: 1.0, 127: 1.7131, 128: 0.0, 129: 0.0044482005007064965, 130: 0.09259999999999996, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.001920347332387049, 135: 2.0100502512562812, 136: 0.0, 137: 0.0067000000000000115, 138: 0.09899999999999998, 139: 2.0381036774479395, 140: 0.09000000000000001, 141: 0.31, 142: 2.0, 143: 0.03947368421052635, 144: 0.02, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0495240191492875, 149: 0.0, 150: 10, 151: 0.038461538461538464, 152: 0.018433179723502304, 153: 0.07623007623007623, 154: 0.0, 155: 0.09090909090909091, 156: 0.011961722488038277, 157: 0.0, 158: 0.03508771929824561, 159: 0.0, 160: 0.011671335200746966, 161: 0.9007803790412486, 162: 0.007518796992481203, 163: 0.06375227686703097, 164: 0.00858000858000858, 165: 0.01668520578420467, 166: 0.056179775280898875, 167: 0.011235955056179775, 168: 0.02425712553062462, 169: 0.03723008190618019, 170: 0.011730205278592375, 171: 0.04040404040404041, 172: 0.01602002503128911, 173: 0.012077294685990338, 174: 0.022911051212938006, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 4.45, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 5.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 1.6, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.072, 201: 10, 202: 0.9000412923264881, 203: 10.0, 204: 9.15211488448582, 205: 9.021928993325746, 206: 9.844713624357173, 207: 0.04269517048974817, 208: 0.9007109140557688, 209: 0.9010953613305983, 210: 10.0, 211: 10.0, 212: 0.9009444988603674, 213: 10.0, 214: 0.8963466442978565, 215: 10.0, 216: 8.899887270330307, 217: 9.699909984159888, 218: 0.9897139073227031, 219: 0.9014817374130921, 220: 10.0, 221: 0.8932058830410452, 222: 0.0037545922629305234, 223: 8.608681744170083, 224: 0.8995062181031812, 225: 0.023856423841067044, 226: 0.007200000000000012, 227: 1.8867568536189265e-05, 228: 0.004046062869592306, 229: 10, 230: 8.93276283618582, 231: 0.0, 232: 0.02267280449896765, 233: 10, 234: 4.5454545454515216e-05, 235: 10.0, 236: 3.333333333332966e-05, 237: 10.0, 238: 10, 239: 0.024042215222249187, 240: 0.0035999999999999366, 241: 0.047044248912042154, 242: 0.01409847240727546, 243: 0.0006662225183210459, 244: 0.03030333333333335, 245: 0.0, 246: 0.0, 247: 0.018656113091617313, 248: 0.0002999999999999947, 249: 8.95107388672361, 250: 8.279933760568172e-06, 251: 10, 252: 0.0, 253: 0.0, 254: 0.7, 255: 10, 256: 10, 257: 0.9983340274885465, 258: 0.0, 259: 0.875, 260: 0.9983340274885465, 261: 0.0, 262: 0.0, 263: 10, 264: 10, 265: 0.94497789971041, 266: 0.0, 267: 0.0, 268: 0.875, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8831948451836937, 277: 0.9154557907410962, 278: 0.9459308604902336, 279: 0.8168395752090845, 280: 0.9940205110645302, 281: 0.6630971030124162, 282: 10, 283: 0.9947131378541612, 284: 0.4008999999999999, 285: 0.970952009132961, 286: 10, 287: 10, 288: 0.9178203645800197, 289: 0.9924561493618224, 290: 0.9851252776098363, 291: 0.8722848147831856, 292: 1.3007347971758478, 293: 10, 294: 0.9983275734795644, 295: 10, 296: 10, 297: 1.0, 298: 0.996738918641727, 299: 0.7162865257480171, 300: 0.9999093901144651, 301: 10, 302: 0.255764106991352, 303: 10, 304: 10, 305: 2.1415492325644014, 306: 10, 307: 0.7499928378163297, 308: 10, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 0.6586914229154579, 312: 2.0, 313: 10, 314: 2.0, 315: 0.0, 316: 0.6816815972832133, 317: 10, 318: 0.0, 319: 3.56479, 320: 10, 321: 0.0, 322: 10, 323: 1.1913485559013017, 324: 10, 325: 3.56479, 326: 0.03679357498680833, 327: 0.9160539215686274, 328: 0.0, 329: 1.562524414412578e-05, 330: 10.0, 331: 3.731769231, 332: 0.0, 333: 0.0, 334: 2.731702619414484, 335: 10.0, 336: 0.0, 337: 0.9995662789950523, 338: 0.004495359127475493, 339: 0.6666666666666666, 340: 0.47664585404127113, 341: 10.0, 342: 0.8573111223287901, 343: 0.08853410740203198, 344: 0.022371902814529648, 345: 0.03868471953578337, 346: 2.0531437839900772, 347: 1.1024737536365443, 348: 10.0, 349: 0.0, 350: 0.008189471379369095, 351: 0.29289321879999997, 352: 0.5774, 353: 5.9571, 354: 0.04290000000000005, 355: 1.3516, 356: 1.3978192384590198, 357: 1.3775763524045956, 358: 1.2929, 359: 6.0, 360: 3.0, 361: 2.5774, 362: 10.0, 363: 2.5, 364: 0.25, 365: 2.232050808, 366: 1.0, 367: 1.0464, 368: 0.6149, 369: 1.5623231915016453, 370: 1.2071, 371: 2.5429, 372: 0.3660000000000001, 373: 8.5926, 374: 7.0429, 375: 6.4571, 376: 0.13826690732881275, 377: 0.6503863231129602, 378: 2.6125159784360585, 379: 5.150265957446808, 380: 0.5907844661783361, 381: 5.855624825931401, 382: 0.2928749660620321, 383: 10, 384: 10.0, 385: 0.25777480887701326, 386: 0.05136677680985275, 387: 10.0, 388: 0.2564392511622064, 389: 10.0, 390: 10.0, 391: 2.6834182121008294, 392: 4.177788344692767, 393: 0.6563101457244982, 394: 0.6546245769151067, 395: 10.0, 396: 10.0, 397: 0.6369840636003921, 398: 0.7754549843379852, 399: 0.6553506806824057, 400: 10.0}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 10, 16: 0.125, 17: 0.0, 18: 10, 19: 10, 20: 0.0, 21: 2.0, 22: 0.0, 23: 0.3333333333333333, 24: 6.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.125, 30: 0.0, 31: 0.16129032258064516, 32: 0.4588235294117647, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.11235955056179775, 37: 0.21333333333333335, 38: 0.0, 39: 0.0, 40: 0.0, 41: 2.1176470588235294, 42: 10, 43: 1.3548387096774193, 44: 0.0, 45: 1.7857142857142858, 46: 10, 47: 10, 48: 10, 49: 1.6, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.19083969465648856, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.3801478352692714, 63: 0.5336481700118064, 64: 2.0, 65: 2.1507936507936507, 66: 0.1295843520782396, 67: 0.0, 68: 0.06870229007633588, 69: 2.6906474820143886, 70: 0.0, 71: 0.020440251572327043, 72: 0.0, 73: 10, 74: 2.0, 75: 7.946666666666666, 76: 0.3854096986644142, 77: 10, 78: 10, 79: 0.5772101972188735, 80: 0.9467914187910013, 81: 0.8989301591490884, 82: 0.9999183637573495, 83: 0.9999990699300358, 84: 0.5377674225061444, 85: 10.0, 86: 0.3358422451203626, 87: 0.6435213709489571, 88: 0.0017165279187326167, 89: 1.0, 90: 10.0, 91: 10, 92: 2.2677298971756623, 93: 0.9999999044979762, 94: 1.0079559050507094, 95: 10.0, 96: 1.0014427149799703, 97: 0.9999999999700772, 98: 0.5075955023281672, 99: 0.7348516181958211, 100: 10, 101: 0.0, 102: 0.8571428571428571, 103: 1.0, 104: 1.0, 105: 0.125, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.2857142857142857, 111: 0.0, 112: 0.0, 113: 10.0, 114: 0.0, 115: 0.0, 116: 10, 117: 10, 118: 1.625, 119: 0.0, 120: 10, 121: 0.0, 122: 1.7777777777777777, 123: 1.75, 124: 0.0, 125: 0.0, 126: 1.0, 127: 1.7131, 128: 0.0, 129: 0.0044482005007064965, 130: 0.09259999999999996, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.001920347332387049, 135: 2.0100502512562812, 136: 0.0, 137: 0.0067000000000000115, 138: 0.09899999999999998, 139: 2.0381036774479395, 140: 0.09000000000000001, 141: 0.31, 142: 2.0, 143: 0.03947368421052635, 144: 0.02, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0495240191492875, 149: 0.0, 150: 10, 151: 0.038461538461538464, 152: 0.018433179723502304, 153: 0.07623007623007623, 154: 0.0, 155: 0.09090909090909091, 156: 0.011961722488038277, 157: 0.0, 158: 0.03508771929824561, 159: 0.0, 160: 0.011671335200746966, 161: 0.9007803790412486, 162: 0.007518796992481203, 163: 0.06375227686703097, 164: 0.00858000858000858, 165: 0.01668520578420467, 166: 0.056179775280898875, 167: 0.011235955056179775, 168: 0.02425712553062462, 169: 0.03723008190618019, 170: 0.011730205278592375, 171: 0.04040404040404041, 172: 0.01602002503128911, 173: 0.012077294685990338, 174: 0.022911051212938006, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 4.45, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 5.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 1.6, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.072, 201: 10, 202: 0.9000412923264881, 203: 10.0, 204: 9.15211488448582, 205: 9.021928993325746, 206: 9.844713624357173, 207: 0.04269517048974817, 208: 0.9007109140557688, 209: 0.9010953613305983, 210: 10.0, 211: 10.0, 212: 0.9009444988603674, 213: 10.0, 214: 0.8963466442978565, 215: 10.0, 216: 8.899887270330307, 217: 9.699909984159888, 218: 0.9897139073227031, 219: 0.9014817374130921, 220: 10.0, 221: 0.8932058830410452, 222: 0.0037545922629305234, 223: 8.608681744170083, 224: 0.8995062181031812, 225: 0.023856423841067044, 226: 0.007200000000000012, 227: 0.0, 228: 0.004046062869592306, 229: 10, 230: 8.93276283618582, 231: 0.0, 232: 0.02267280449896765, 233: 10, 234: 0.0, 235: 10.0, 236: 0.0, 237: 10.0, 238: 10, 239: 0.024042215222249187, 240: 0.0035999999999999366, 241: 0.047044248912042154, 242: 0.01409847240727546, 243: 0.0, 244: 0.03030333333333335, 245: 0.0, 246: 0.0, 247: 0.018656113091617313, 248: 0.0, 249: 8.95107388672361, 250: 0.0, 251: 10, 252: 0.0, 253: 0.0, 254: 0.7, 255: 10, 256: 10, 257: 0.9983340274885465, 258: 0.0, 259: 0.875, 260: 0.9983340274885465, 261: 0.0, 262: 0.0, 263: 10, 264: 10, 265: 0.94497789971041, 266: 0.0, 267: 0.0, 268: 0.875, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8831948451836937, 277: 0.9154557907410962, 278: 0.9459308604902336, 279: 0.8168395752090845, 280: 0.9940205110645302, 281: 0.6630971030124162, 282: 10, 283: 0.9947131378541612, 284: 0.4008999999999999, 285: 0.970952009132961, 286: 10, 287: 10, 288: 0.9178203645800197, 289: 0.9924561493618224, 290: 0.9851252776098363, 291: 0.8722848147831856, 292: 1.3007347971758478, 293: 10, 294: 0.9983275734795644, 295: 10, 296: 10, 297: 1.0, 298: 0.996738918641727, 299: 0.7162865257480171, 300: 0.9999093901144651, 301: 10, 302: 0.255764106991352, 303: 10, 304: 10, 305: 2.1415492325644014, 306: 10, 307: 0.7499928378163297, 308: 10, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 0.6586914229154579, 312: 2.0, 313: 10, 314: 2.0, 315: 0.0, 316: 0.6816815972832133, 317: 10, 318: 0.0, 319: 3.56479, 320: 10, 321: 0.0, 322: 10, 323: 1.1913485559013017, 324: 10, 325: 3.56479, 326: 0.03679357498680833, 327: 0.9160539215686274, 328: 0.0, 329: 0.0, 330: 10.0, 331: 3.731769231, 332: 0.0, 333: 0.0, 334: 2.731702619414484, 335: 10.0, 336: 0.0, 337: 0.9995662789950523, 338: 0.004495359127475493, 339: 0.6666666666666666, 340: 0.47664585404127113, 341: 10.0, 342: 0.8573111223287901, 343: 0.08853410740203198, 344: 0.022371902814529648, 345: 0.03868471953578337, 346: 2.0531437839900772, 347: 1.1024737536365443, 348: 10.0, 349: 0.0, 350: 0.008189471379369095, 351: 0.29289321879999997, 352: 0.5774, 353: 5.9571, 354: 0.04290000000000005, 355: 1.3516, 356: 1.3978192384590198, 357: 1.3775763524045956, 358: 1.2929, 359: 6.0, 360: 3.0, 361: 2.5774, 362: 10.0, 363: 2.5, 364: 0.25, 365: 2.232050808, 366: 1.0, 367: 1.0464, 368: 0.6149, 369: 1.5623231915016453, 370: 1.2071, 371: 2.5429, 372: 0.3660000000000001, 373: 8.5926, 374: 7.0429, 375: 6.4571, 376: 0.13826690732881275, 377: 0.6503863231129602, 378: 2.6125159784360585, 379: 5.150265957446808, 380: 0.5907844661783361, 381: 5.855624825931401, 382: 0.2928749660620321, 383: 10, 384: 10.0, 385: 0.25777480887701326, 386: 0.05136677680985275, 387: 10.0, 388: 0.2564392511622064, 389: 10.0, 390: 10.0, 391: 2.6834182121008294, 392: 4.177788344692767, 393: 0.6563101457244982, 394: 0.6546245769151067, 395: 10.0, 396: 10.0, 397: 0.6369840636003921, 398: 0.7754549843379852, 399: 0.6553506806824057, 400: 10.0}</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 2.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 2.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 2.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0042796005706134095, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.12330456226880394, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.02512562814070352, 75: 0.0, 76: 0.5580353709046836, 77: 2.0721460433057406e-06, 78: 0.03710144890073974, 79: 0.37935473888119864, 80: 0.8521123689751403, 81: 2.0166665144143125e-07, 82: 6.441695647843136e-05, 83: 0.904673364662762, 84: 3.5562671880997904e-06, 85: 0.9000000201740207, 86: 0.5977420358893716, 87: 2.4519742724293225e-05, 88: 0.4939132861388031, 89: 0.9969306549411275, 90: 2.129838963792373, 91: 10.0, 92: 1.1409569074580963, 93: 10.0, 94: 2.012450530513992, 95: 10.0, 96: 0.0, 97: 9.785145636478187, 98: 4.899134063392434, 99: 1.3338131396936082e-11, 100: 3.1249234106049903, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 2.3333333333333335, 117: 0.0, 118: 0.0, 119: 0.0, 120: 2.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.014800000000000035, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.003840694664774098, 135: 0.0, 136: 0.0, 137: 0.013400000000000009, 138: 0.19799999999999995, 139: 0.038103677447939716, 140: 0.0, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.37999999999999995, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0035842293906809273, 150: 0.0, 151: 0.016025641025641024, 152: 0.007680491551459293, 153: 0.00693000693000693, 154: 0.0, 155: 0.0, 156: 0.011961722488038277, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.018674136321195144, 161: 0.016722408026755852, 162: 0.042606516290726815, 163: 0.015938069216757743, 164: 0.00429000429000429, 165: 0.0055617352614015575, 166: 0.0, 167: 0.0, 168: 0.01212856276531231, 169: 0.007446016381236039, 170: 0.005865102639296188, 171: 0.006734006734006734, 172: 0.0, 173: 0.012077294685990338, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.010278977910098222, 202: 0.00042600646578766515, 203: 0.9009808195128701, 204: 0.011816070885064598, 205: 0.0054969071862006145, 206: 0.0024826735664252374, 207: 0.990011017765239, 208: 0.9007635966188348, 209: 0.8992138239783832, 210: 0.8986244154747128, 211: 0.900224502185595, 212: 0.0026266859009538646, 213: 0.8997851743801331, 214: 0.9002341035068896, 215: 0.9017537150262984, 216: 0.9011771295393746, 217: 0.8984743004167536, 218: 0.8998764716895982, 219: 0.9008925670066309, 220: 0.004950620922591317, 221: 0.014714128623879481, 222: 0.9902138547451488, 223: 0.9014750721702491, 224: 0.8998337851526617, 225: 0.8996618520670573, 226: 1.8072, 227: 0.4339729439067187, 228: 0.12854030501089322, 229: 0.0037000000000000366, 230: 0.2359413202933985, 231: 0.23076923076923078, 232: 0.05085067508245728, 233: 0.0, 234: 3.5455, 235: 6.2821, 236: 0.6667, 237: 0.05320961939026702, 238: 0.02439024390243894, 239: 0.19231079880461996, 240: 0.5636, 241: 0.047044248912042154, 242: 0.07043039072909245, 243: 0.2597527574209786, 244: 0.3333333333333333, 245: 0.047619047619047616, 246: 0.0, 247: 0.15304480392987216, 248: 0.8352999999999999, 249: 0.17074384277303256, 250: 0.2800057599539204, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.9858392336526447, 258: 0.0, 259: 0.83984375, 260: 0.9858392336526447, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.83984375, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8717703599584733, 277: 0.9068381698570855, 278: 0.8276675253056633, 279: 0.4430137591052903, 280: 0.8063957873500192, 281: 0.8119658694916937, 282: 0.08063730222209968, 283: 0.8399731034216174, 284: 1.2504, 285: 0.8837852587960782, 286: 0.8945001696107706, 287: 0.6728095460133102, 288: 0.9278859763760179, 289: 0.5058204591063679, 290: 0.9247284013362598, 291: 0.2949958504952033, 292: 1.2337258962081012, 293: 2.030749401583502, 294: 10.0, 295: 0.14268193386455702, 296: 0.9315223507373115, 297: 0.4229566968558609, 298: 0.9581766315801489, 299: 0.41484816903873545, 300: 0.9941728420172972, 301: 0.6321230180627598, 302: 0.255764106991352, 303: 0.5361138605413154, 304: 1.0, 305: 0.10241450498159957, 306: 0.0, 307: 0.0450421773038358, 308: 2.2424764413821054, 309: 0.7293273785356611, 310: 0.26424603612551967, 311: 0.46387419365848664, 312: 4.0, 313: 0.4621197859236748, 314: 2.14, 315: 0.0, 316: 0.674132487412055, 317: 0.00043200472931489395, 318: 0.0, 319: 3.14148, 320: 0.0, 321: 0.0, 322: 1.0, 323: 1.1913485559013017, 324: 0.5361138605413154, 325: 3.14148, 326: 0.9835886703692773, 327: 0.0006127450980392157, 328: 0.0, 329: 0.06248535133361467, 330: 0.010199999999999987, 331: 0.0047000000000000375, 332: 0.0, 333: 0.0, 334: 3.694722650231125, 335: 10.0, 336: 0.0, 337: 0.9001477864165007, 338: 0.004787100025195156, 339: 0.013333333333333334, 340: 9.182244545777124, 341: 0.41957268401064474, 342: 0.07925290257445734, 343: 0.0, 344: 0.097907144575415, 345: 0.03868471953578337, 346: 0.0018128041217441205, 347: 1.0, 348: 2.6863, 349: 0.0, 350: 0.0006000000000000449, 351: 0.0, 352: 0.8425999999999999, 353: 6.781186547732965e-06, 354: 0.15892540399838606, 355: 6.781186548621143e-06, 356: 1.7071, 357: 1.8198140984931586, 358: 1.7071, 359: 0.0, 360: 2.0, 361: 0.8425999999999999, 362: 1.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 1.5, 367: 0.18350240799999995, 368: 1.0, 369: 0.18018590150684144, 370: 1.5, 371: 0.29290000000000005, 372: 0.134, 373: 1.7726, 374: 1.2071, 375: 1.7071, 376: 0.34956176724067844, 377: 0.04884103066111944, 378: 1.7788584449508145, 379: 0.16888297872340424, 380: 0.22764660146499152, 381: 0.28542965486213767, 382: 0.22427502036278074, 383: 0.2506444457766321, 384: 1.0339552866027906, 385: 0.4844503822459735, 386: 0.5019525382997897, 387: 2.321983223984719, 388: 0.31466949936606925, 389: 0.036344605308157044, 390: 0.10542759008790474, 391: 0.03910829249543579, 392: 0.5773234004332435, 393: 0.031069562826505297, 394: 0.03612626925467985, 395: 0.027158492095662814, 396: 0.4213630872006254, 397: 0.2739681272007842, 398: 0.3263649530139555, 399: 0.033947957952783055, 400: 0.43474596029340556}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 2.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 2.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 2.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0042796005706134095, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.12330456226880394, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.02512562814070352, 75: 0.0, 76: 0.5580353709046836, 77: 2.0721460433057406e-06, 78: 0.03710144890073974, 79: 0.37935473888119864, 80: 0.8521123689751403, 81: 2.0166665144143125e-07, 82: 6.441695647843136e-05, 83: 0.904673364662762, 84: 3.5562671880997904e-06, 85: 0.9000000201740207, 86: 0.5977420358893716, 87: 2.4519742724293225e-05, 88: 0.4939132861388031, 89: 0.9969306549411275, 90: 2.129838963792373, 91: 10.0, 92: 1.1409569074580963, 93: 10.0, 94: 2.012450530513992, 95: 10.0, 96: 0.0, 97: 9.785145636478187, 98: 4.899134063392434, 99: 1.3338131396936082e-11, 100: 3.1249234106049903, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 2.3333333333333335, 117: 0.0, 118: 0.0, 119: 0.0, 120: 2.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.014800000000000035, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.003840694664774098, 135: 0.0, 136: 0.0, 137: 0.013400000000000009, 138: 0.19799999999999995, 139: 0.038103677447939716, 140: 0.0, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.37999999999999995, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0035842293906809273, 150: 0.0, 151: 0.016025641025641024, 152: 0.007680491551459293, 153: 0.00693000693000693, 154: 0.0, 155: 0.0, 156: 0.011961722488038277, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.018674136321195144, 161: 0.016722408026755852, 162: 0.042606516290726815, 163: 0.015938069216757743, 164: 0.00429000429000429, 165: 0.0055617352614015575, 166: 0.0, 167: 0.0, 168: 0.01212856276531231, 169: 0.007446016381236039, 170: 0.005865102639296188, 171: 0.006734006734006734, 172: 0.0, 173: 0.012077294685990338, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.010278977910098222, 202: 0.00042600646578766515, 203: 0.9009808195128701, 204: 0.011816070885064598, 205: 0.0054969071862006145, 206: 0.0024826735664252374, 207: 0.990011017765239, 208: 0.9007635966188348, 209: 0.8992138239783832, 210: 0.8986244154747128, 211: 0.900224502185595, 212: 0.0026266859009538646, 213: 0.8997851743801331, 214: 0.9002341035068896, 215: 0.9017537150262984, 216: 0.9011771295393746, 217: 0.8984743004167536, 218: 0.8998764716895982, 219: 0.9008925670066309, 220: 0.004950620922591317, 221: 0.014714128623879481, 222: 0.9902138547451488, 223: 0.9014750721702491, 224: 0.8998337851526617, 225: 0.8996618520670573, 226: 1.8072, 227: 0.4339729439067187, 228: 0.12854030501089322, 229: 0.0037000000000000366, 230: 0.2359413202933985, 231: 0.23076923076923078, 232: 0.05085067508245728, 233: 0.0, 234: 3.5455, 235: 6.2821, 236: 0.6667, 237: 0.05320961939026702, 238: 0.02439024390243894, 239: 0.19231079880461996, 240: 0.5636, 241: 0.047044248912042154, 242: 0.07043039072909245, 243: 0.2597527574209786, 244: 0.3333333333333333, 245: 0.047619047619047616, 246: 0.0, 247: 0.15304480392987216, 248: 0.8352999999999999, 249: 0.17074384277303256, 250: 0.2800057599539204, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.9858392336526447, 258: 0.0, 259: 0.83984375, 260: 0.9858392336526447, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.83984375, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8717703599584733, 277: 0.9068381698570855, 278: 0.8276675253056633, 279: 0.4430137591052903, 280: 0.8063957873500192, 281: 0.8119658694916937, 282: 0.08063730222209968, 283: 0.8399731034216174, 284: 1.2504, 285: 0.8837852587960782, 286: 0.8945001696107706, 287: 0.6728095460133102, 288: 0.9278859763760179, 289: 0.5058204591063679, 290: 0.9247284013362598, 291: 0.2949958504952033, 292: 1.2337258962081012, 293: 2.030749401583502, 294: 10.0, 295: 0.14268193386455702, 296: 0.9315223507373115, 297: 0.4229566968558609, 298: 0.9581766315801489, 299: 0.41484816903873545, 300: 0.9941728420172972, 301: 0.6321230180627598, 302: 0.255764106991352, 303: 0.5361138605413154, 304: 1.0, 305: 0.10241450498159957, 306: 0.0, 307: 0.0450421773038358, 308: 2.2424764413821054, 309: 0.7293273785356611, 310: 0.26424603612551967, 311: 0.46387419365848664, 312: 4.0, 313: 0.4621197859236748, 314: 2.14, 315: 0.0, 316: 0.674132487412055, 317: 0.00043200472931489395, 318: 0.0, 319: 3.14148, 320: 0.0, 321: 0.0, 322: 1.0, 323: 1.1913485559013017, 324: 0.5361138605413154, 325: 3.14148, 326: 0.9835886703692773, 327: 0.0006127450980392157, 328: 0.0, 329: 0.06248535133361467, 330: 0.010199999999999987, 331: 0.0047000000000000375, 332: 0.0, 333: 0.0, 334: 3.694722650231125, 335: 10.0, 336: 0.0, 337: 0.9001477864165007, 338: 0.004787100025195156, 339: 0.013333333333333334, 340: 9.182244545777124, 341: 0.41957268401064474, 342: 0.07925290257445734, 343: 0.0, 344: 0.097907144575415, 345: 0.03868471953578337, 346: 0.0018128041217441205, 347: 1.0, 348: 2.6863, 349: 0.0, 350: 0.0, 351: 0.0, 352: 0.8425999999999999, 353: 0.0, 354: 0.15892540399838606, 355: 0.0, 356: 1.7071, 357: 1.8198140984931586, 358: 1.7071, 359: 0.0, 360: 2.0, 361: 0.8425999999999999, 362: 1.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 1.5, 367: 0.18350240799999995, 368: 1.0, 369: 0.18018590150684144, 370: 1.5, 371: 0.29290000000000005, 372: 0.134, 373: 1.7726, 374: 1.2071, 375: 1.7071, 376: 0.34956176724067844, 377: 0.04884103066111944, 378: 1.7788584449508145, 379: 0.16888297872340424, 380: 0.22764660146499152, 381: 0.28542965486213767, 382: 0.22427502036278074, 383: 0.2506444457766321, 384: 1.0339552866027906, 385: 0.4844503822459735, 386: 0.5019525382997897, 387: 2.321983223984719, 388: 0.31466949936606925, 389: 0.036344605308157044, 390: 0.10542759008790474, 391: 0.03910829249543579, 392: 0.5773234004332435, 393: 0.031069562826505297, 394: 0.03612626925467985, 395: 0.027158492095662814, 396: 0.4213630872006254, 397: 0.2739681272007842, 398: 0.3263649530139555, 399: 0.033947957952783055, 400: 0.43474596029340556}</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 2.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.007132667617689016, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.10559662090813093, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.04830917874396135, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.3401360544217687, 74: 0.25125628140703515, 75: 0.04666666666666667, 76: 0.8999991211800807, 77: 0.8994581638542156, 78: 0.8666082248661258, 79: 0.38233537552305136, 80: 0.8929284320392084, 81: 0.8989635357437258, 82: 0.00043458792466549554, 83: 0.9208573970542847, 84: 0.4583061203633767, 85: 0.9000107509235608, 86: 0.899999638238093, 87: 0.9579166665776754, 88: 0.9006975292543979, 89: 0.8753058704820322, 90: 2.12982124626951, 91: 2.2655474711880643, 92: 1.1145167404918224, 93: 6.2905064139014, 94: 1.9882459721847427, 95: 10.0, 96: 0.8991065220524124, 97: 0.027982258020706356, 98: 0.5343423124865065, 99: 0.9999989984223738, 100: 2.191214947083338, 101: 0.0, 102: 2.0, 103: 1.5, 104: 0.0, 105: 1.75, 106: 1.2, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 3.3333333333333335, 117: 0.1, 118: 0.0, 119: 0.0, 120: 2.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0131, 128: 0.0, 129: 0.0036394367733052564, 130: 0.003999999999999948, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.003840694664774098, 135: 0.010050251256281305, 136: 1.0131391483299035, 137: 0.013400000000000009, 138: 0.009000000000000008, 139: 0.0, 140: 0.09000000000000001, 141: 0.3, 142: 2.0, 143: 0.019736842105263174, 144: 0.02, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.00641025641025641, 152: 0.030721966205837174, 153: 0.00693000693000693, 154: 0.0, 155: 0.055658627087198514, 156: 0.004784688995215311, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.014005602240896359, 161: 0.011148272017837236, 162: 0.012531328320802004, 163: 0.015938069216757743, 164: 0.00858000858000858, 165: 0.0055617352614015575, 166: 0.0, 167: 0.0, 168: 0.002425712553062462, 169: 0.007446016381236039, 170: 0.002932551319648094, 171: 0.010101010101010102, 172: 0.025031289111389236, 173: 0.012077294685990338, 174: 0.013477088948787063, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.9990218584267595, 202: 0.9899819750124469, 203: 0.9006009315816432, 204: 0.9025964496119852, 205: 0.018270610564655614, 206: 0.9901781445092249, 207: 0.9990202018686841, 208: 0.9011681313676606, 209: 0.018609796637064566, 210: 0.9898819798594378, 211: 0.9990613700766493, 212: 0.9990082576153303, 213: 0.8988753843880941, 214: 0.9003323848212017, 215: 0.9014974421556976, 216: 0.05250705681964215, 217: 0.9008533144260219, 218: 0.9034317440515184, 219: 0.9901372737475833, 220: 0.9010856014822193, 221: 0.014815041866599507, 222: 0.989900419795361, 223: 0.9990112129053976, 224: 0.9898006627893616, 225: 0.989760621139767, 226: 0.0007900000000000129, 227: 0.003792381275824944, 228: 0.0005664488017429538, 229: 0.0037000000000000366, 230: 0.2359413202933985, 231: 0.0, 232: 0.05085067508245728, 233: 0.0, 234: 0.009500000000000008, 235: 0.018900000000000028, 236: 1.3333, 237: 8.467903806097329, 238: 0.0, 239: 8.692270414344561, 240: 0.006399999999999961, 241: 0.047044248912042154, 242: 0.008459083444365221, 243: 0.2597527574209786, 244: 0.02666666666666669, 245: 0.047619047619047616, 246: 0.0, 247: 0.02600152451935307, 248: 0.0002999999999999947, 249: 0.17074384277303256, 250: 7.999936000404534e-06, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.9, 255: 0.0, 256: 0.0, 257: 0.9900041649312786, 258: 0.0, 259: 0.9375, 260: 0.9900041649312786, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.8888888888888888, 266: 0.0, 267: 0.0, 268: 0.9375, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.8, 274: 0.0, 275: 0.0, 276: 10, 277: 0.9872707522641213, 278: 10.0, 279: 0.23689696612954655, 280: 0.9648992107450955, 281: 10, 282: 0.39526160465565274, 283: 10.0, 284: 0.31117736557, 285: 10.0, 286: 0.9356315860956502, 287: 10.0, 288: 0.8949370760638059, 289: 0.9924547735835905, 290: 10.0, 291: 0.6666907535018974, 292: 0.13058107933221186, 293: 0.942966918308476, 294: 2.72875758899652, 295: 0.7197904926463387, 296: 10.0, 297: 10.0, 298: 0.9951406626680374, 299: 0.547379056317075, 300: 5.446829928887369, 301: 0.6321230180627598, 302: 0.255764106991352, 303: 0.6586914229154579, 304: 0.32533085938239586, 305: 0.027735391796068508, 306: 0.0, 307: 0.27327709692821894, 308: 0.6816708886411997, 309: 0.6321180132629585, 310: 0.81606150903138, 311: 4.607665790648769e-05, 312: 10, 313: 0.4621197859236748, 314: 0.0, 315: 0.0, 316: 0.18027987587095265, 317: 0.045042177303835786, 318: 0.0, 319: 10.0, 320: 0.0, 321: 0.0, 322: 1.4669624095260332, 323: 1.1913485559013017, 324: 0.6586914229154579, 325: 10.0, 326: 0.009193921994759107, 327: 0.0012254901960784314, 328: 0.0, 329: 0.06248535133361467, 330: 0.01319999999999999, 331: 0.0006000000000000449, 332: 0.0, 333: 0.0, 334: 0.5739358628659476, 335: 10.0, 336: 0.0, 337: 0.9059949881128317, 338: 0.0078105316200555485, 339: 0.0, 340: 0.01659794018923114, 341: 0.06393676851816228, 342: 0.10095911155981828, 343: 0.0007256894049346726, 344: 0.097907144575415, 345: 1.0764023210831721, 346: 0.027573704799160357, 347: 1.0100106611734518, 348: 0.006699999999999984, 349: 0.0, 350: 0.0010999999999999899, 351: 3.0, 352: 0.5774, 353: 6.781000000066761e-06, 354: 0.29290000000000005, 355: 1.2071, 356: 1.2929, 357: 1.0, 358: 1.7071, 359: 0.0, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 1.5, 367: 1.0, 368: 0.0, 369: 0.4226661278217193, 370: 1.5, 371: 2.7071, 372: 0.134, 373: 10, 374: 1.4142067809999999, 375: 5.0429, 376: 0.34956176724067844, 377: 0.04884103066111944, 378: 0.11154337798032575, 379: 0.38519503546099293, 380: 0.02303883455415959, 381: 0.0711913790517814, 382: 0.2928749660620321, 383: 0.4987111084467359, 384: 1.5015663442289768, 385: 0.4844503822459735, 386: 2.1045358966656655, 387: 0.6609916119923596, 388: 0.1422175010565513, 389: 1.6944959738012084, 390: 0.43015155337356653, 391: 0.6922780586114535, 392: 0.056691498916891236, 393: 0.031069562826505297, 394: 0.03612626925467985, 395: 0.6813944061613293, 396: 0.06602231540046903, 397: 0.9239844629179219, 398: 0.3263649530139555, 399: 0.033947957952783055, 400: 0.25002241790562957}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 2.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.007132667617689016, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.10559662090813093, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.04830917874396135, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.3401360544217687, 74: 0.25125628140703515, 75: 0.04666666666666667, 76: 0.8999991211800807, 77: 0.8994581638542156, 78: 0.8666082248661258, 79: 0.38233537552305136, 80: 0.8929284320392084, 81: 0.8989635357437258, 82: 0.00043458792466549554, 83: 0.9208573970542847, 84: 0.4583061203633767, 85: 0.9000107509235608, 86: 0.899999638238093, 87: 0.9579166665776754, 88: 0.9006975292543979, 89: 0.8753058704820322, 90: 2.12982124626951, 91: 2.2655474711880643, 92: 1.1145167404918224, 93: 6.2905064139014, 94: 1.9882459721847427, 95: 10.0, 96: 0.8991065220524124, 97: 0.027982258020706356, 98: 0.5343423124865065, 99: 0.9999989984223738, 100: 2.191214947083338, 101: 0.0, 102: 2.0, 103: 1.5, 104: 0.0, 105: 1.75, 106: 1.2, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 3.3333333333333335, 117: 0.1, 118: 0.0, 119: 0.0, 120: 2.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0131, 128: 0.0, 129: 0.0036394367733052564, 130: 0.003999999999999948, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.003840694664774098, 135: 0.010050251256281305, 136: 1.0131391483299035, 137: 0.013400000000000009, 138: 0.009000000000000008, 139: 0.0, 140: 0.09000000000000001, 141: 0.3, 142: 2.0, 143: 0.019736842105263174, 144: 0.02, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.00641025641025641, 152: 0.030721966205837174, 153: 0.00693000693000693, 154: 0.0, 155: 0.055658627087198514, 156: 0.004784688995215311, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.014005602240896359, 161: 0.011148272017837236, 162: 0.012531328320802004, 163: 0.015938069216757743, 164: 0.00858000858000858, 165: 0.0055617352614015575, 166: 0.0, 167: 0.0, 168: 0.002425712553062462, 169: 0.007446016381236039, 170: 0.002932551319648094, 171: 0.010101010101010102, 172: 0.025031289111389236, 173: 0.012077294685990338, 174: 0.013477088948787063, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.9990218584267595, 202: 0.9899819750124469, 203: 0.9006009315816432, 204: 0.9025964496119852, 205: 0.018270610564655614, 206: 0.9901781445092249, 207: 0.9990202018686841, 208: 0.9011681313676606, 209: 0.018609796637064566, 210: 0.9898819798594378, 211: 0.9990613700766493, 212: 0.9990082576153303, 213: 0.8988753843880941, 214: 0.9003323848212017, 215: 0.9014974421556976, 216: 0.05250705681964215, 217: 0.9008533144260219, 218: 0.9034317440515184, 219: 0.9901372737475833, 220: 0.9010856014822193, 221: 0.014815041866599507, 222: 0.989900419795361, 223: 0.9990112129053976, 224: 0.9898006627893616, 225: 0.989760621139767, 226: 0.0, 227: 0.003792381275824944, 228: 0.0, 229: 0.0037000000000000366, 230: 0.2359413202933985, 231: 0.0, 232: 0.05085067508245728, 233: 0.0, 234: 0.009500000000000008, 235: 0.018900000000000028, 236: 1.3333, 237: 8.467903806097329, 238: 0.0, 239: 8.692270414344561, 240: 0.006399999999999961, 241: 0.047044248912042154, 242: 0.008459083444365221, 243: 0.2597527574209786, 244: 0.02666666666666669, 245: 0.047619047619047616, 246: 0.0, 247: 0.02600152451935307, 248: 0.0, 249: 0.17074384277303256, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.9, 255: 0.0, 256: 0.0, 257: 0.9900041649312786, 258: 0.0, 259: 0.9375, 260: 0.9900041649312786, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.8888888888888888, 266: 0.0, 267: 0.0, 268: 0.9375, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.8, 274: 0.0, 275: 0.0, 276: 10, 277: 0.9872707522641213, 278: 10.0, 279: 0.23689696612954655, 280: 0.9648992107450955, 281: 10, 282: 0.39526160465565274, 283: 10.0, 284: 0.31117736557, 285: 10.0, 286: 0.9356315860956502, 287: 10.0, 288: 0.8949370760638059, 289: 0.9924547735835905, 290: 10.0, 291: 0.6666907535018974, 292: 0.13058107933221186, 293: 0.942966918308476, 294: 2.72875758899652, 295: 0.7197904926463387, 296: 10.0, 297: 10.0, 298: 0.9951406626680374, 299: 0.547379056317075, 300: 5.446829928887369, 301: 0.6321230180627598, 302: 0.255764106991352, 303: 0.6586914229154579, 304: 0.32533085938239586, 305: 0.027735391796068508, 306: 0.0, 307: 0.27327709692821894, 308: 0.6816708886411997, 309: 0.6321180132629585, 310: 0.81606150903138, 311: 0.0, 312: 10, 313: 0.4621197859236748, 314: 0.0, 315: 0.0, 316: 0.18027987587095265, 317: 0.045042177303835786, 318: 0.0, 319: 10.0, 320: 0.0, 321: 0.0, 322: 1.4669624095260332, 323: 1.1913485559013017, 324: 0.6586914229154579, 325: 10.0, 326: 0.009193921994759107, 327: 0.0012254901960784314, 328: 0.0, 329: 0.06248535133361467, 330: 0.01319999999999999, 331: 0.0, 332: 0.0, 333: 0.0, 334: 0.5739358628659476, 335: 10.0, 336: 0.0, 337: 0.9059949881128317, 338: 0.0078105316200555485, 339: 0.0, 340: 0.01659794018923114, 341: 0.06393676851816228, 342: 0.10095911155981828, 343: 0.0007256894049346726, 344: 0.097907144575415, 345: 1.0764023210831721, 346: 0.027573704799160357, 347: 1.0100106611734518, 348: 0.006699999999999984, 349: 0.0, 350: 0.0010999999999999899, 351: 3.0, 352: 0.5774, 353: 0.0, 354: 0.29290000000000005, 355: 1.2071, 356: 1.2929, 357: 1.0, 358: 1.7071, 359: 0.0, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 1.5, 367: 1.0, 368: 0.0, 369: 0.4226661278217193, 370: 1.5, 371: 2.7071, 372: 0.134, 373: 10, 374: 1.4142067809999999, 375: 5.0429, 376: 0.34956176724067844, 377: 0.04884103066111944, 378: 0.11154337798032575, 379: 0.38519503546099293, 380: 0.02303883455415959, 381: 0.0711913790517814, 382: 0.2928749660620321, 383: 0.4987111084467359, 384: 1.5015663442289768, 385: 0.4844503822459735, 386: 2.1045358966656655, 387: 0.6609916119923596, 388: 0.1422175010565513, 389: 1.6944959738012084, 390: 0.43015155337356653, 391: 0.6922780586114535, 392: 0.056691498916891236, 393: 0.031069562826505297, 394: 0.03612626925467985, 395: 0.6813944061613293, 396: 0.06602231540046903, 397: 0.9239844629179219, 398: 0.3263649530139555, 399: 0.033947957952783055, 400: 0.25002241790562957}</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.12330456226880394, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.0, 79: 0.024406796288053607, 80: 0.0, 81: 0.0, 82: 0.0, 83: 0.06293687015023787, 84: 0.0, 85: 0.0, 86: 6.915669215143585e-06, 87: 0.0, 88: 0.0, 89: 0.0, 90: 3.6595171205469496e-06, 91: 5.474319326328318e-09, 92: 0.0, 93: 8.838882770251795e-10, 94: 0.0, 95: 7.675541320538696e-10, 96: 0.0, 97: 0.007480719167673525, 98: 1.2247835158174887e-10, 99: 2.6676529556500105e-05, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0010000000000000009, 141: 0.0, 142: 0.0, 143: 0.03289473684210529, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.006688963210702341, 162: 0.0, 163: 0.0, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.015018773466833541, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0015337240471062976, 202: 0.00026066097272970745, 203: 0.8999195249800218, 204: 0.010446981050640791, 205: 0.0030204804965681237, 206: 0.00029135622427262217, 207: 0.8999892358188681, 208: 0.0003643979777032649, 209: 0.0009000603820310566, 210: 0.0032388421147387238, 211: 0.000438367452839529, 212: 0.0019469155656806193, 213: 0.02840937347880817, 214: 0.9002438627034594, 215: 0.005287319901959047, 216: 0.006218460167803234, 217: 0.9015538554098826, 218: 0.0038080339777700443, 219: 0.0013146165834667589, 220: 0.004366689408929374, 221: 0.0005839286914300915, 222: 0.0005467256375535835, 223: 0.9000865779449159, 224: 0.00022239707498451972, 225: 0.0007666115162274202, 226: 0.0002999999999999947, 227: 0.0, 228: 0.0027886710239650283, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.0, 233: 0.0, 234: 0.0, 235: 0.0, 236: 3.333333333332966e-05, 237: 0.010604052262828893, 238: 0.0, 239: 0.0, 240: 0.0, 241: 0.0, 242: 0.0, 243: 0.013028351469390822, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 8.858486541492782, 277: 5.512816933358927, 278: 0.7290179979292196, 279: 10.0, 280: 10.0, 281: 0.39910012838482467, 282: 0.019637587224535912, 283: 10.0, 284: 0.018299999999999983, 285: 0.14082198470611704, 286: 10.0, 287: 0.4571208299775336, 288: 10.0, 289: 10.0, 290: 10.0, 291: 0.07305099183018347, 292: 7.158405590785557, 293: 0.4730227705149449, 294: 0.045158860482984155, 295: 8.110470836055963, 296: 7.783459892144146, 297: 10.0, 298: 10.0, 299: 1.7844056038631966, 300: 10.0, 301: 0.26424603612551967, 302: 0.5953916913504904, 303: 3.4130857708677813e-06, 304: 1.9466648995588542, 305: 0.003479916861003096, 306: 0.0, 307: 0.0004774789113481002, 308: 6.079643327595279e-05, 309: 0.00013533631073209444, 310: 0.6321230180627598, 311: 3.4130857708677813e-06, 312: 2.0, 313: 5.378802140798489e-06, 314: 0.0, 315: 0.0, 316: 0.31380291586158443, 317: 2.7284509219826816e-05, 318: 0.0, 319: 0.2816073464102068, 320: 0.0, 321: 0.0, 322: 4.326574354094551e-05, 323: 0.999978086514441, 324: 3.4130857708677813e-06, 325: 0.2816073464102068, 326: 0.8370225286862887, 327: 5.025735294117647, 328: 0.0, 329: 0.0, 330: 0.010599999999999943, 331: 0.4053, 332: 0.0, 333: 0.0823045267489712, 334: 0.875, 335: 0.0, 336: 0.8333333333333334, 337: 0.0, 338: 0.0, 339: 0.4, 340: 0.1538268269084545, 341: 2.227221096235431e-05, 342: 0.0, 343: 0.0, 344: 0.03500120279047392, 345: 0.019342359767891684, 346: 0.21714531056196928, 347: 0.9046186371767767, 348: 0.0, 349: 1.1666666666666667, 350: 0.0012999999999999678, 351: 0.0, 352: 0.4226, 353: 0.0, 354: 0.20709999999999995, 355: 0.20709999999999995, 356: 0.0, 357: 0.4226661278217193, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 0.0, 364: 1.0, 365: 1.0, 366: 0.0, 367: 0.5, 368: 1.0, 369: 0.0, 370: 0.0, 371: 9.999999999998899e-05, 372: 0.366, 373: 1.5774000000000001, 374: 1.4142, 375: 0.29290000000000005, 376: 0.0005853944094834694, 377: 0.3496136768870398, 378: 0.004168287667426132, 379: 0.02051473847517723, 380: 0.001483406310103527, 381: 0.0036848983439381026, 382: 0.0017583099538443997, 383: 0.004271326659073093, 384: 0.0001222512568957215, 385: 0.0002597788168929343, 386: 0.0007509762691498788, 387: 0.0, 388: 0.0023187015271448736, 389: 0.004321557004135068, 390: 0.0024644402615799027, 391: 0.0006566093334614866, 392: 0.003127806836794029, 393: 0.0005842727522683649, 394: 0.00024176279615947536, 395: 0.000583704904742682, 396: 0.3551631014142563, 397: 0.0005808254982393087, 398: 0.09153577563462041, 399: 0.0007582285024986241, 400: 0.0025466740795207533}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.12330456226880394, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.0, 79: 0.024406796288053607, 80: 0.0, 81: 0.0, 82: 0.0, 83: 0.06293687015023787, 84: 0.0, 85: 0.0, 86: 6.915669215143585e-06, 87: 0.0, 88: 0.0, 89: 0.0, 90: 3.6595171205469496e-06, 91: 5.474319326328318e-09, 92: 0.0, 93: 8.838882770251795e-10, 94: 0.0, 95: 7.675541320538696e-10, 96: 0.0, 97: 0.007480719167673525, 98: 1.2247835158174887e-10, 99: 2.6676529556500105e-05, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0010000000000000009, 141: 0.0, 142: 0.0, 143: 0.03289473684210529, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.006688963210702341, 162: 0.0, 163: 0.0, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.015018773466833541, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0015337240471062976, 202: 0.00026066097272970745, 203: 0.8999195249800218, 204: 0.010446981050640791, 205: 0.0030204804965681237, 206: 0.00029135622427262217, 207: 0.8999892358188681, 208: 0.0003643979777032649, 209: 0.0009000603820310566, 210: 0.0032388421147387238, 211: 0.000438367452839529, 212: 0.0019469155656806193, 213: 0.02840937347880817, 214: 0.9002438627034594, 215: 0.005287319901959047, 216: 0.006218460167803234, 217: 0.9015538554098826, 218: 0.0038080339777700443, 219: 0.0013146165834667589, 220: 0.004366689408929374, 221: 0.0005839286914300915, 222: 0.0005467256375535835, 223: 0.9000865779449159, 224: 0.00022239707498451972, 225: 0.0007666115162274202, 226: 0.0, 227: 0.0, 228: 0.0027886710239650283, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.0, 233: 0.0, 234: 0.0, 235: 0.0, 236: 0.0, 237: 0.010604052262828893, 238: 0.0, 239: 0.0, 240: 0.0, 241: 0.0, 242: 0.0, 243: 0.013028351469390822, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 8.858486541492782, 277: 5.512816933358927, 278: 0.7290179979292196, 279: 10.0, 280: 10.0, 281: 0.39910012838482467, 282: 0.019637587224535912, 283: 10.0, 284: 0.018299999999999983, 285: 0.14082198470611704, 286: 10.0, 287: 0.4571208299775336, 288: 10.0, 289: 10.0, 290: 10.0, 291: 0.07305099183018347, 292: 7.158405590785557, 293: 0.4730227705149449, 294: 0.045158860482984155, 295: 8.110470836055963, 296: 7.783459892144146, 297: 10.0, 298: 10.0, 299: 1.7844056038631966, 300: 10.0, 301: 0.26424603612551967, 302: 0.5953916913504904, 303: 0.0, 304: 1.9466648995588542, 305: 0.003479916861003096, 306: 0.0, 307: 0.0004774789113481002, 308: 0.0, 309: 0.0, 310: 0.6321230180627598, 311: 0.0, 312: 2.0, 313: 0.0, 314: 0.0, 315: 0.0, 316: 0.31380291586158443, 317: 0.0, 318: 0.0, 319: 0.2816073464102068, 320: 0.0, 321: 0.0, 322: 0.0, 323: 0.999978086514441, 324: 0.0, 325: 0.2816073464102068, 326: 0.8370225286862887, 327: 5.025735294117647, 328: 0.0, 329: 0.0, 330: 0.010599999999999943, 331: 0.4053, 332: 0.0, 333: 0.0823045267489712, 334: 0.875, 335: 0.0, 336: 0.8333333333333334, 337: 0.0, 338: 0.0, 339: 0.4, 340: 0.1538268269084545, 341: 2.227221096235431e-05, 342: 0.0, 343: 0.0, 344: 0.03500120279047392, 345: 0.019342359767891684, 346: 0.21714531056196928, 347: 0.9046186371767767, 348: 0.0, 349: 1.1666666666666667, 350: 0.0012999999999999678, 351: 0.0, 352: 0.4226, 353: 0.0, 354: 0.20709999999999995, 355: 0.20709999999999995, 356: 0.0, 357: 0.4226661278217193, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 0.4226, 362: 1.0, 363: 0.0, 364: 1.0, 365: 1.0, 366: 0.0, 367: 0.5, 368: 1.0, 369: 0.0, 370: 0.0, 371: 0.0, 372: 0.366, 373: 1.5774000000000001, 374: 1.4142, 375: 0.29290000000000005, 376: 0.0005853944094834694, 377: 0.3496136768870398, 378: 0.004168287667426132, 379: 0.02051473847517723, 380: 0.001483406310103527, 381: 0.0036848983439381026, 382: 0.0017583099538443997, 383: 0.004271326659073093, 384: 0.0, 385: 0.0, 386: 0.0007509762691498788, 387: 0.0, 388: 0.0023187015271448736, 389: 0.004321557004135068, 390: 0.0024644402615799027, 391: 0.0006566093334614866, 392: 0.003127806836794029, 393: 0.0005842727522683649, 394: 0.0, 395: 0.000583704904742682, 396: 0.3551631014142563, 397: 0.0005808254982393087, 398: 0.09153577563462041, 399: 0.0007582285024986241, 400: 0.0025466740795207533}</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 2.251256281407035, 75: 0.0, 76: 0.0, 77: 5.172218863554254e-12, 78: 0.3339130403337495, 79: 2.463342378689302e-08, 80: 9.944758356135059e-08, 81: 1.0083483824328928e-10, 82: 4.627106447758086e-11, 83: 2.7073156646108907e-08, 84: 0.9000000000283106, 85: 3.3428147400234197e-10, 86: 2.766267686057434e-07, 87: 5.769385166805269e-07, 88: 0.0, 89: 3.055155236444597e-07, 90: 3.6595171205469496e-07, 91: 0.0, 92: 0.0, 93: 1.039747243207286e-05, 94: 4.799385945207027e-07, 95: 8.391157622990254e-06, 96: 2.805920771652534e-08, 97: 6.657833394738208e-08, 98: 9.859507302330785e-08, 99: 0.0013338131263554767, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 2.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 2.0, 140: 0.0, 141: 0.0, 142: 2.0, 143: 0.0, 144: 0.0, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.004553734061930784, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.9000375156830588, 202: 0.999000399840064, 203: 0.9000555955305906, 204: 0.0002598504868220378, 205: 0.007452025502010074, 206: 0.8995921532211741, 207: 0.900229359572685, 208: 0.9002134987935262, 209: 0.00026041677267784913, 210: 0.899708219573986, 211: 0.9002079915110051, 212: 0.9900523213487542, 213: 0.9004917269107292, 214: 0.990002471009921, 215: 0.0028226147185741123, 216: 0.8994271772852601, 217: 0.8996290657088357, 218: 0.9006640965484581, 219: 0.0020423995073723953, 220: 0.00015886823719692323, 221: 0.00011633787479003466, 222: 0.0016433565547781365, 223: 0.9002065866556493, 224: 0.9001151151835154, 225: 0.8996524213995457, 226: 2.8915662650591534e-05, 227: 1.867889285104983e-05, 228: 0.0, 229: 1.5789473684191258e-05, 230: 0.0, 231: 0.0, 232: 3.3898190174644294e-06, 233: 10.0, 234: 4.499999999996174e-05, 235: 4.871794871796897e-05, 236: 3.333333333332966e-05, 237: 0.0, 238: 0.0, 239: 0.0, 240: 3.636363636361217e-05, 241: 0.0006035386423557106, 242: 8.450632811496482e-06, 243: 0.0006662225183210459, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 6.476476476474646e-05, 249: 1.463393218638913e-05, 250: 0.0007919936640506004, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.937722370062396, 277: 10.0, 278: 0.39540465339543823, 279: 0.5088906874647439, 280: 10.0, 281: 0.8317376372817415, 282: 0.07564516277316556, 283: 10.0, 284: 1.2544, 285: 0.6994249988383354, 286: 0.33706970519910123, 287: 0.07274225340172116, 288: 0.41631708924336597, 289: 0.9742199796017947, 290: 0.5096011662976776, 291: 0.9175215668413327, 292: 2.385595962210431, 293: 10.0, 294: 0.6233778755329246, 295: 0.9634546201400127, 296: 10.0, 297: 1.3052225277410485, 298: 10.0, 299: 0.19331896037359084, 301: 0.6321230180627598, 302: 10, 303: 0.005353915705964376, 304: 10, 305: 0.00155063666116652, 306: 0.0, 307: 2.9493423457881523e-05, 309: 7.592222310214164e-06, 310: 6.684891643700028e-06, 311: 10, 312: 0.0, 313: 10, 314: 2.14159, 315: 0.0, 316: 1.6301305697054862, 317: 2.9510077755850075e-05, 318: 0.0, 319: 0.00379999999999997, 320: 0.0, 321: 0.0, 322: 4.326574354094551e-05, 323: 3.191348555901302, 324: 0.005353915705964376, 325: 0.00379999999999997, 326: 6.5125432642000485, 327: 0.04411764705882353, 328: 0.0, 329: 0.0, 330: 0.021094736842105277, 331: 0.29469999999999996, 332: 0.0, 333: 0.0, 334: 0.2639637904468413, 335: 2.222222222214576e-05, 336: 0.0, 337: 0.6063740923986378, 338: 0.029982363315696564, 339: 0.0, 340: 1.7631592287018863e-05, 341: 0.029246112655542767, 342: 0.05047955577990914, 343: 0.0, 344: 0.06146259321626163, 345: 0.01160541586073501, 347: 10.0, 348: 0.0, 349: 0.0, 350: 0.0006000000000000449, 351: 0.0, 352: 0.4074, 353: 0.29290000000000005, 354: 1.2071, 355: 0.965919045102521, 356: 0.7071, 358: 0.2928999999999998, 359: 2.0, 360: 0.0, 361: 0.577254, 362: 0.0, 363: 1.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 1.0, 368: 0.0, 369: 0.9999155359788988, 370: 0.366, 371: 1.7070999999999998, 372: 0.0, 374: 1.4142067811865475, 375: 1.7070999999999998, 376: 4.878286745697985e-05, 377: 0.0011537251337271819, 378: 0.0048352136942145015, 379: 0.02994791666666663, 380: 0.0025371363096943996, 381: 0.0005784433446879458, 382: 0.08244663658577575, 383: 0.001139020442419527, 384: 0.005180397010956775, 385: 0.000148445038224581, 386: 0.0027035145689397236, 387: 0.0, 388: 0.004009183428708485, 389: 0.0009638004829365489, 390: 0.0018046688529679317, 391: 0.0009288619839210475, 392: 0.03767105193638722, 393: 0.0005499037668408948, 394: 0.0001381501692339421, 395: 0.0005674908796109809, 396: 0.00042640892616014063, 397: 0.0017424764947180874, 398: 0.00259349493089621, 399: 0.00017232465965885473, 400: 0.004447712476909545}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 2.251256281407035, 75: 0.0, 76: 0.0, 77: 5.172218863554254e-12, 78: 0.3339130403337495, 79: 2.463342378689302e-08, 80: 9.944758356135059e-08, 81: 1.0083483824328928e-10, 82: 4.627106447758086e-11, 83: 2.7073156646108907e-08, 84: 0.9000000000283106, 85: 3.3428147400234197e-10, 86: 2.766267686057434e-07, 87: 5.769385166805269e-07, 88: 0.0, 89: 3.055155236444597e-07, 90: 3.6595171205469496e-07, 91: 0.0, 92: 0.0, 93: 1.039747243207286e-05, 94: 4.799385945207027e-07, 95: 8.391157622990254e-06, 96: 2.805920771652534e-08, 97: 6.657833394738208e-08, 98: 9.859507302330785e-08, 99: 0.0013338131263554767, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 2.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 2.0, 140: 0.0, 141: 0.0, 142: 2.0, 143: 0.0, 144: 0.0, 145: 0.4, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.004553734061930784, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.9000375156830588, 202: 0.999000399840064, 203: 0.9000555955305906, 204: 0.0002598504868220378, 205: 0.007452025502010074, 206: 0.8995921532211741, 207: 0.900229359572685, 208: 0.9002134987935262, 209: 0.00026041677267784913, 210: 0.899708219573986, 211: 0.9002079915110051, 212: 0.9900523213487542, 213: 0.9004917269107292, 214: 0.990002471009921, 215: 0.0028226147185741123, 216: 0.8994271772852601, 217: 0.8996290657088357, 218: 0.9006640965484581, 219: 0.0020423995073723953, 220: 0.00015886823719692323, 221: 0.00011633787479003466, 222: 0.0016433565547781365, 223: 0.9002065866556493, 224: 0.9001151151835154, 225: 0.8996524213995457, 226: 0.0, 227: 0.0, 228: 0.0, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.0, 233: 10.0, 234: 0.0, 235: 0.0, 236: 0.0, 237: 0.0, 238: 0.0, 239: 0.0, 240: 0.0, 241: 0.0006035386423557106, 242: 0.0, 243: 0.0, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 0.0, 249: 0.0, 250: 0.0007919936640506004, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.937722370062396, 277: 10.0, 278: 0.39540465339543823, 279: 0.5088906874647439, 280: 10.0, 281: 0.8317376372817415, 282: 0.07564516277316556, 283: 10.0, 284: 1.2544, 285: 0.6994249988383354, 286: 0.33706970519910123, 287: 0.07274225340172116, 288: 0.41631708924336597, 289: 0.9742199796017947, 290: 0.5096011662976776, 291: 0.9175215668413327, 292: 2.385595962210431, 293: 10.0, 294: 0.6233778755329246, 295: 0.9634546201400127, 296: 10.0, 297: 1.3052225277410485, 298: 10.0, 299: 0.19331896037359084, 301: 0.6321230180627598, 302: 10, 303: 0.005353915705964376, 304: 10, 305: 0.00155063666116652, 306: 0.0, 307: 0.0, 309: 0.0, 310: 0.0, 311: 10, 312: 0.0, 313: 10, 314: 2.14159, 315: 0.0, 316: 1.6301305697054862, 317: 0.0, 318: 0.0, 319: 0.00379999999999997, 320: 0.0, 321: 0.0, 322: 0.0, 323: 3.191348555901302, 324: 0.005353915705964376, 325: 0.00379999999999997, 326: 6.5125432642000485, 327: 0.04411764705882353, 328: 0.0, 329: 0.0, 330: 0.021094736842105277, 331: 0.29469999999999996, 332: 0.0, 333: 0.0, 334: 0.2639637904468413, 335: 0.0, 336: 0.0, 337: 0.6063740923986378, 338: 0.029982363315696564, 339: 0.0, 340: 0.0, 341: 0.029246112655542767, 342: 0.05047955577990914, 343: 0.0, 344: 0.06146259321626163, 345: 0.01160541586073501, 347: 10.0, 348: 0.0, 349: 0.0, 350: 0.0, 351: 0.0, 352: 0.4074, 353: 0.29290000000000005, 354: 1.2071, 355: 0.965919045102521, 356: 0.7071, 358: 0.2928999999999998, 359: 2.0, 360: 0.0, 361: 0.577254, 362: 0.0, 363: 1.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 1.0, 368: 0.0, 369: 0.9999155359788988, 370: 0.366, 371: 1.7070999999999998, 372: 0.0, 374: 1.4142067811865475, 375: 1.7070999999999998, 376: 0.0, 377: 0.0011537251337271819, 378: 0.0048352136942145015, 379: 0.02994791666666663, 380: 0.0025371363096943996, 381: 0.0005784433446879458, 382: 0.08244663658577575, 383: 0.001139020442419527, 384: 0.005180397010956775, 385: 0.0, 386: 0.0027035145689397236, 387: 0.0, 388: 0.004009183428708485, 389: 0.0009638004829365489, 390: 0.0018046688529679317, 391: 0.0009288619839210475, 392: 0.03767105193638722, 393: 0.0005499037668408948, 394: 0.0, 395: 0.0005674908796109809, 396: 0.00042640892616014063, 397: 0.0017424764947180874, 398: 0.00259349493089621, 399: 0.0, 400: 0.004447712476909545}</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.0, 79: 0.0, 80: 1.000438042127193e-09, 81: 0.0, 82: 0.0, 83: 4.8431407238119694e-11, 84: 0.9000000000556639, 85: 0.0, 86: 2.766267686057434e-07, 87: 0.0, 88: 8.843568238832642e-08, 89: 3.063972439648985e-06, 90: 2.561661984382865e-07, 91: 3.7109194197773815e-05, 92: 0.0, 93: 2.3275724628329725e-07, 94: 4.778149724210535e-07, 95: 2.6608543244534147e-08, 96: 2.805920771652534e-08, 97: 5.984569343584906e-08, 98: 9.859507302330785e-08, 99: 0.0013338130063122943, 100: 4.664064791947747e-10, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.009999999999999995, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 3.501698323678827e-05, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.004553734061930784, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.9002067878513279, 202: 0.00037039413980056074, 203: 0.8999053041598183, 204: 0.9001290267143032, 205: 0.8997974667521104, 206: 0.9000315765747519, 207: 0.9006194674568946, 208: 0.9001192812901502, 209: 0.9001666016012433, 210: 0.8997618014327166, 211: 0.8999581674235116, 212: 0.8999793150760849, 213: 0.0002754301721090843, 214: 0.9900016934304222, 215: 0.9000752028866211, 216: 0.8986952557297619, 217: 0.017880926067888093, 218: 0.8999324799904715, 219: 0.9018692320866534, 220: 0.0005889386086597131, 221: 0.9002256208331767, 222: 0.9001033112381731, 223: 0.8998146066716743, 224: 0.9001013179077522, 225: 0.9003211297826487, 226: 9.999999999998899e-05, 227: 0.0, 228: 0.0, 229: 0.0, 230: 0.0, 231: 0.0, 232: 3.3898190174644294e-06, 233: 0.0, 234: 4.5454499999986187e-05, 235: 0.0, 236: 3.3333400000001845e-05, 237: 0.0, 238: 0.0, 239: 0.0, 240: 0.0, 241: 0.01175312093008479, 242: 0.0, 243: 0.028121170248640796, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 7.874217248038722, 277: 10.0, 278: 10.0, 279: 10.0, 280: 10.0, 281: 6.019056649172902, 282: 0.03516562319000471, 283: 10.0, 284: 1.2000000000000002, 285: 10.0, 286: 10.0, 287: 0.6856534271544231, 288: 10.0, 289: 10.0, 290: 10.0, 291: 0.040996523466781766, 292: 10.0, 293: 0.6754336218007734, 294: 0.06759667967278811, 295: 8.117869813662416, 296: 10.0, 297: 10.0, 298: 10.0, 299: 10.0, 300: 10.0, 301: 0.6321230180627598, 302: 0.40461128559308157, 303: 3.4130857708677813e-06, 304: 0.05333510044114582, 305: 0.008796337851180351, 306: 0.0, 307: 2.9493423457881523e-05, 308: 3.877059711229717e-06, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 3.4130857708677813e-06, 312: 0.0, 313: 0.26894548584030337, 314: 0.0, 315: 0.0, 316: 0.03750570876515022, 317: 4.092676382974023e-05, 318: 0.0, 319: 3.2829800000000002, 320: 0.0, 321: 0.0, 322: 0.4669191437824923, 323: 1.1913397905070782, 324: 3.4130857708677813e-06, 325: 3.2829800000000002, 326: 0.5823508894314614, 327: 0.007352941176470588, 328: 0.0, 329: 0.0, 330: 0.005199999999999982, 331: 0.0, 332: 0.0, 333: 0.0, 334: 0.9622496147919877, 335: 0.0, 336: 0.16666666666666666, 337: 0.0002248923729358093, 338: 6.298815822624653e-05, 339: 0.0, 340: 0.14736264438621127, 341: 0.004499661529884864, 342: 0.24280666330136294, 343: 0.0, 344: 0.04182703872985326, 345: 0.027079303675048357, 346: 0.39613586489838754, 347: 0.9184420230931859, 348: 0.0, 349: 0.0, 350: 0.0012999999999999678, 351: 1.5, 352: 0.4074, 353: 0.29290000000000005, 354: 1.4141, 355: 0.9571, 356: 0.20709999999999995, 357: 0.4226661278217193, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 0.4226, 362: 0.0, 363: 0.5, 364: 1.0, 365: 0.0, 366: 0.0, 367: 2.0, 368: 1.0, 369: 0.4226661278217193, 370: 0.0, 371: 9.999999999998899e-05, 372: 0.0, 373: 2.4581, 374: 1.7071, 375: 9.999999999998899e-05, 376: 0.0009268744816820395, 377: 0.009229801069817765, 378: 0.01172678263769238, 379: 0.1439494680851064, 380: 0.0008082006792979015, 381: 0.34849069134691607, 382: 0.08463159527842067, 383: 0.08846891673161082, 384: 0.31829642873515784, 385: 0.00011133377866851816, 386: 0.3496395313908081, 387: 2.321983223984719, 388: 0.26738169482232804, 389: 0.0008187122381933769, 390: 0.15974230104981274, 391: 0.00011210403254222237, 392: 0.350768743065462, 393: 0.0012716524608194454, 394: 0.0015196518615735164, 395: 0.0005674908796109809, 396: 0.0, 397: 0.40857443641775876, 398: 0.31714738012102983, 399: 0.0011373427537480125, 400: 0.4155741673989849}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.0, 79: 0.0, 80: 1.000438042127193e-09, 81: 0.0, 82: 0.0, 83: 4.8431407238119694e-11, 84: 0.9000000000556639, 85: 0.0, 86: 2.766267686057434e-07, 87: 0.0, 88: 8.843568238832642e-08, 89: 3.063972439648985e-06, 90: 2.561661984382865e-07, 91: 3.7109194197773815e-05, 92: 0.0, 93: 2.3275724628329725e-07, 94: 4.778149724210535e-07, 95: 2.6608543244534147e-08, 96: 2.805920771652534e-08, 97: 5.984569343584906e-08, 98: 9.859507302330785e-08, 99: 0.0013338130063122943, 100: 4.664064791947747e-10, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.009999999999999995, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.004553734061930784, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.9002067878513279, 202: 0.00037039413980056074, 203: 0.8999053041598183, 204: 0.9001290267143032, 205: 0.8997974667521104, 206: 0.9000315765747519, 207: 0.9006194674568946, 208: 0.9001192812901502, 209: 0.9001666016012433, 210: 0.8997618014327166, 211: 0.8999581674235116, 212: 0.8999793150760849, 213: 0.0002754301721090843, 214: 0.9900016934304222, 215: 0.9000752028866211, 216: 0.8986952557297619, 217: 0.017880926067888093, 218: 0.8999324799904715, 219: 0.9018692320866534, 220: 0.0005889386086597131, 221: 0.9002256208331767, 222: 0.9001033112381731, 223: 0.8998146066716743, 224: 0.9001013179077522, 225: 0.9003211297826487, 226: 0.0, 227: 0.0, 228: 0.0, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.0, 233: 0.0, 234: 0.0, 235: 0.0, 236: 0.0, 237: 0.0, 238: 0.0, 239: 0.0, 240: 0.0, 241: 0.01175312093008479, 242: 0.0, 243: 0.028121170248640796, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 7.874217248038722, 277: 10.0, 278: 10.0, 279: 10.0, 280: 10.0, 281: 6.019056649172902, 282: 0.03516562319000471, 283: 10.0, 284: 1.2000000000000002, 285: 10.0, 286: 10.0, 287: 0.6856534271544231, 288: 10.0, 289: 10.0, 290: 10.0, 291: 0.040996523466781766, 292: 10.0, 293: 0.6754336218007734, 294: 0.06759667967278811, 295: 8.117869813662416, 296: 10.0, 297: 10.0, 298: 10.0, 299: 10.0, 300: 10.0, 301: 0.6321230180627598, 302: 0.40461128559308157, 303: 0.0, 304: 0.05333510044114582, 305: 0.008796337851180351, 306: 0.0, 307: 0.0, 308: 0.0, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 0.0, 312: 0.0, 313: 0.26894548584030337, 314: 0.0, 315: 0.0, 316: 0.03750570876515022, 317: 0.0, 318: 0.0, 319: 3.2829800000000002, 320: 0.0, 321: 0.0, 322: 0.4669191437824923, 323: 1.1913397905070782, 324: 0.0, 325: 3.2829800000000002, 326: 0.5823508894314614, 327: 0.007352941176470588, 328: 0.0, 329: 0.0, 330: 0.005199999999999982, 331: 0.0, 332: 0.0, 333: 0.0, 334: 0.9622496147919877, 335: 0.0, 336: 0.16666666666666666, 337: 0.0002248923729358093, 338: 0.0, 339: 0.0, 340: 0.14736264438621127, 341: 0.004499661529884864, 342: 0.24280666330136294, 343: 0.0, 344: 0.04182703872985326, 345: 0.027079303675048357, 346: 0.39613586489838754, 347: 0.9184420230931859, 348: 0.0, 349: 0.0, 350: 0.0012999999999999678, 351: 1.5, 352: 0.4074, 353: 0.29290000000000005, 354: 1.4141, 355: 0.9571, 356: 0.20709999999999995, 357: 0.4226661278217193, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 0.4226, 362: 0.0, 363: 0.5, 364: 1.0, 365: 0.0, 366: 0.0, 367: 2.0, 368: 1.0, 369: 0.4226661278217193, 370: 0.0, 371: 0.0, 372: 0.0, 373: 2.4581, 374: 1.7071, 375: 0.0, 376: 0.0009268744816820395, 377: 0.009229801069817765, 378: 0.01172678263769238, 379: 0.1439494680851064, 380: 0.0008082006792979015, 381: 0.34849069134691607, 382: 0.08463159527842067, 383: 0.08846891673161082, 384: 0.31829642873515784, 385: 0.0, 386: 0.3496395313908081, 387: 2.321983223984719, 388: 0.26738169482232804, 389: 0.0008187122381933769, 390: 0.15974230104981274, 391: 0.0, 392: 0.350768743065462, 393: 0.0012716524608194454, 394: 0.0015196518615735164, 395: 0.0005674908796109809, 396: 0.0, 397: 0.40857443641775876, 398: 0.31714738012102983, 399: 0.0011373427537480125, 400: 0.4155741673989849}</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>{0: 1.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.8, 36: 1.1235955056179776, 37: 0.5333333333333333, 38: 0.0, 39: 0.0, 40: 1.3924050632911393, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.40160642570281124, 55: 1.1363636363636365, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.9100310237849017, 60: 0.0, 61: 0.0, 62: 0.12671594508975711, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.14492753623188406, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.034013605442176874, 74: 0.0, 75: 0.0, 76: 0.17436643703099663, 77: 0.0, 78: 0.033391304010665764, 79: 2.4633423786893023e-09, 80: 1.0105434768961546e-07, 81: 0.0, 82: 0.734494844065125, 83: 0.8370634832098619, 84: 6.838317831169677e-10, 85: 6.685629480046839e-10, 86: 6.91587668522004e-05, 87: 0.0, 88: 0.0, 89: 1.000000030246298, 90: 3.62292194934148e-06, 91: 0.01798831468979882, 92: 4.6836884998092206e-11, 93: 0.9689550407959244, 94: 0.0, 95: 0.8744140232514492, 96: 0.4676590537212988, 97: 8.37839708101887e-09, 98: 1.0222473254670867, 99: 1.3338131396936083e-09, 100: 4.664158073243586e-05, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.009999999999999995, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.004668534080298786, 161: 0.006688963210702341, 162: 0.03759398496240601, 163: 0.00546448087431694, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.025031289111389236, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.405, 181: 0.0, 182: 0.81, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.02211064279537443, 202: 0.9000390594602, 203: 0.9001718968860597, 204: 9.266872440160284, 205: 0.001972871997555737, 206: 0.0007613693846411125, 207: 0.006565277991102006, 208: 0.000684559323332294, 209: 0.0006311530223029693, 210: 0.8990034048020872, 211: 0.01810551533051416, 212: 0.00014256683940040124, 213: 0.0023510343911260366, 214: 0.0013901313781966233, 215: 0.9001171310086528, 216: 0.012445515770712536, 217: 0.8984995663653897, 218: 0.9003118000998371, 219: 0.08161727535063301, 220: 10.0, 221: 0.0006212826396784409, 222: 0.8995819700315344, 223: 0.8995107881830514, 224: 0.0014517945613041411, 225: 0.002816006550948262, 226: 0.0015000000000000013, 227: 0.0, 228: 0.9001307189542483, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.9000071186199369, 233: 0.0, 234: 0.0, 235: 0.00029999999999996696, 236: 3.333333333321864e-05, 237: 0.07252414315470555, 238: 0.4878048780487804, 239: 0.025119134157176422, 240: 0.000500000000000056, 241: 0.14116451192782947, 242: 0.1126948222972764, 243: 0.008290769116885113, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.013212501058694044, 248: 0.0006000000000000172, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 10.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.9876543209876543, 266: 0.0, 267: 0.0, 268: 10.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 10.0, 277: 10.0, 278: 10.0, 279: 10.0, 280: 10.0, 281: 0.3415675736614241, 282: 0.053608038907429365, 283: 10.0, 284: 0.0010000000000000009, 285: 10.0, 286: 10.0, 287: 0.5224555974736127, 288: 10.0, 289: 10.0, 290: 10.0, 291: 10.0, 292: 0.03300116474699117, 293: 10.0, 294: 0.052995676343421984, 295: 4.446942686611673, 296: 10.0, 297: 10.0, 298: 10.0, 299: 10.0, 300: 10.0, 301: 0.6321230180627598, 302: 10, 303: 3.4130857708677813e-06, 304: 2.135997879470625, 305: 0.9048110582532987, 306: 0.0, 307: 0.27327709692821894, 308: 0.6212382206910528, 309: 0.7293273785356611, 310: 0.1036309458117205, 311: 3.4130857708677813e-06, 312: 0.0, 313: 0.2689449940943321, 314: 0.0, 315: 0.0, 316: 0.31380291586158443, 317: 1.2282349196243831, 318: 0.0, 319: 0.4232, 320: 0.0, 321: 0.0, 322: 0.9338815533085252, 323: 1.1913485559013017, 324: 3.4130857708677813e-06, 325: 0.4232, 326: 0.07530430271971954, 327: 0.004595588235294118, 328: 0.0, 329: 0.0, 330: 0.08420000000000005, 331: 0.00019999999999997797, 332: 0.0, 333: 0.205761316872428, 334: 0.9626829738058552, 335: 10.0, 336: 0.0, 337: 0.03623979952451327, 338: 0.004661123708742663, 339: 0.3333333333333333, 340: 0.1545409063960805, 341: 0.06749154837085526, 342: 0.07824331145885917, 343: 0.005805515239477509, 344: 0.007006254510464373, 345: 0.030947775628626693, 346: 1.289857837992558, 347: 0.7211470699842792, 348: 0.002599999999999991, 349: 0.5555555555555556, 350: 0.0018000000000000238, 351: 1.5, 352: 0.4074, 353: 0.20709999999999995, 354: 1.7071, 355: 0.20709999999999995, 356: 0.20709999999999995, 357: 0.4226661278217193, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 4.5926, 362: 0.0, 363: 0.5, 364: 1.0, 365: 1.0, 366: 1.5, 367: 1.0, 368: 0.0, 369: 1.8866693608914036, 370: 0.5, 371: 1.7071, 372: 1.366, 373: 1.5774000000000001, 374: 0.7071, 375: 0.20709999999999995, 376: 0.04879912841276818, 377: 0.3511170156976541, 378: 0.003723670316234175, 379: 0.05927249556737591, 380: 0.3402115644309859, 381: 0.1385907406217194, 382: 0.3075361681771756, 383: 0.49853126311372215, 384: 0.34422897660416574, 385: 0.33381577970756326, 386: 0.3496395313908081, 387: 0.0, 388: 0.27057990382528635, 389: 0.3448954846465547, 390: 0.10484543884501181, 391: 0.20949040709778682, 392: 0.27606065409203784, 393: 0.34533956557602424, 394: 0.32852110243835053, 395: 0.24181597081475484, 396: 0.35470115841091604, 397: 0.10407666896576766, 398: 0.2798841347719185, 399: 0.31118387041185597, 400: 0.15132983016194693}</t>
+          <t>{0: 1.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.8, 36: 1.1235955056179776, 37: 0.5333333333333333, 38: 0.0, 39: 0.0, 40: 1.3924050632911393, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.40160642570281124, 55: 1.1363636363636365, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.9100310237849017, 60: 0.0, 61: 0.0, 62: 0.12671594508975711, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.14492753623188406, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.034013605442176874, 74: 0.0, 75: 0.0, 76: 0.17436643703099663, 77: 0.0, 78: 0.033391304010665764, 79: 2.4633423786893023e-09, 80: 1.0105434768961546e-07, 81: 0.0, 82: 0.734494844065125, 83: 0.8370634832098619, 84: 6.838317831169677e-10, 85: 6.685629480046839e-10, 86: 6.91587668522004e-05, 87: 0.0, 88: 0.0, 89: 1.000000030246298, 90: 3.62292194934148e-06, 91: 0.01798831468979882, 92: 4.6836884998092206e-11, 93: 0.9689550407959244, 94: 0.0, 95: 0.8744140232514492, 96: 0.4676590537212988, 97: 8.37839708101887e-09, 98: 1.0222473254670867, 99: 1.3338131396936083e-09, 100: 4.664158073243586e-05, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.009999999999999995, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.019230769230769232, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.004668534080298786, 161: 0.006688963210702341, 162: 0.03759398496240601, 163: 0.00546448087431694, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.025031289111389236, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.405, 181: 0.0, 182: 0.81, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.02211064279537443, 202: 0.9000390594602, 203: 0.9001718968860597, 204: 9.266872440160284, 205: 0.001972871997555737, 206: 0.0007613693846411125, 207: 0.006565277991102006, 208: 0.000684559323332294, 209: 0.0006311530223029693, 210: 0.8990034048020872, 211: 0.01810551533051416, 212: 0.00014256683940040124, 213: 0.0023510343911260366, 214: 0.0013901313781966233, 215: 0.9001171310086528, 216: 0.012445515770712536, 217: 0.8984995663653897, 218: 0.9003118000998371, 219: 0.08161727535063301, 220: 10.0, 221: 0.0006212826396784409, 222: 0.8995819700315344, 223: 0.8995107881830514, 224: 0.0014517945613041411, 225: 0.002816006550948262, 226: 0.0015000000000000013, 227: 0.0, 228: 0.9001307189542483, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.9000071186199369, 233: 0.0, 234: 0.0, 235: 0.0, 236: 0.0, 237: 0.07252414315470555, 238: 0.4878048780487804, 239: 0.025119134157176422, 240: 0.0, 241: 0.14116451192782947, 242: 0.1126948222972764, 243: 0.008290769116885113, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.013212501058694044, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 10.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.9876543209876543, 266: 0.0, 267: 0.0, 268: 10.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 10.0, 277: 10.0, 278: 10.0, 279: 10.0, 280: 10.0, 281: 0.3415675736614241, 282: 0.053608038907429365, 283: 10.0, 284: 0.0010000000000000009, 285: 10.0, 286: 10.0, 287: 0.5224555974736127, 288: 10.0, 289: 10.0, 290: 10.0, 291: 10.0, 292: 0.03300116474699117, 293: 10.0, 294: 0.052995676343421984, 295: 4.446942686611673, 296: 10.0, 297: 10.0, 298: 10.0, 299: 10.0, 300: 10.0, 301: 0.6321230180627598, 302: 10, 303: 0.0, 304: 2.135997879470625, 305: 0.9048110582532987, 306: 0.0, 307: 0.27327709692821894, 308: 0.6212382206910528, 309: 0.7293273785356611, 310: 0.1036309458117205, 311: 0.0, 312: 0.0, 313: 0.2689449940943321, 314: 0.0, 315: 0.0, 316: 0.31380291586158443, 317: 1.2282349196243831, 318: 0.0, 319: 0.4232, 320: 0.0, 321: 0.0, 322: 0.9338815533085252, 323: 1.1913485559013017, 324: 0.0, 325: 0.4232, 326: 0.07530430271971954, 327: 0.004595588235294118, 328: 0.0, 329: 0.0, 330: 0.08420000000000005, 331: 0.0, 332: 0.0, 333: 0.205761316872428, 334: 0.9626829738058552, 335: 10.0, 336: 0.0, 337: 0.03623979952451327, 338: 0.004661123708742663, 339: 0.3333333333333333, 340: 0.1545409063960805, 341: 0.06749154837085526, 342: 0.07824331145885917, 343: 0.005805515239477509, 344: 0.007006254510464373, 345: 0.030947775628626693, 346: 1.289857837992558, 347: 0.7211470699842792, 348: 0.002599999999999991, 349: 0.5555555555555556, 350: 0.0018000000000000238, 351: 1.5, 352: 0.4074, 353: 0.20709999999999995, 354: 1.7071, 355: 0.20709999999999995, 356: 0.20709999999999995, 357: 0.4226661278217193, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 4.5926, 362: 0.0, 363: 0.5, 364: 1.0, 365: 1.0, 366: 1.5, 367: 1.0, 368: 0.0, 369: 1.8866693608914036, 370: 0.5, 371: 1.7071, 372: 1.366, 373: 1.5774000000000001, 374: 0.7071, 375: 0.20709999999999995, 376: 0.04879912841276818, 377: 0.3511170156976541, 378: 0.003723670316234175, 379: 0.05927249556737591, 380: 0.3402115644309859, 381: 0.1385907406217194, 382: 0.3075361681771756, 383: 0.49853126311372215, 384: 0.34422897660416574, 385: 0.33381577970756326, 386: 0.3496395313908081, 387: 0.0, 388: 0.27057990382528635, 389: 0.3448954846465547, 390: 0.10484543884501181, 391: 0.20949040709778682, 392: 0.27606065409203784, 393: 0.34533956557602424, 394: 0.32852110243835053, 395: 0.24181597081475484, 396: 0.35470115841091604, 397: 0.10407666896576766, 398: 0.2798841347719185, 399: 0.31118387041185597, 400: 0.15132983016194693}</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.0, 79: 0.0, 80: 0.0, 81: 0.0, 82: 0.0, 83: 0.0, 84: 0.0, 85: 0.0, 86: 6.915669215143584e-05, 87: 0.0, 88: 0.0, 89: 0.0, 90: 0.0, 91: 0.0, 92: 0.0, 93: 0.0, 94: 0.0, 95: 0.0, 96: 0.0, 97: 7.480711679481134e-10, 98: 0.0, 99: 1.3338131396936082e-10, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0010000000000000009, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.09, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.014005602240896359, 161: 0.016722408026755852, 162: 0.0, 163: 0.0, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.013477088948787063, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0050079506900020535, 202: 0.9000326050810861, 203: 0.0037008145159081996, 204: 0.004355903868126497, 205: 0.003983511774317081, 206: 0.899790857127425, 207: 0.9004704527702285, 208: 8.927920118437973, 209: 0.0011148140796962557, 210: 0.0002394825185443977, 211: 0.9016077433184178, 212: 0.002180588921159467, 213: 0.9000347542692952, 214: 0.8997696181148409, 215: 0.004550314182209536, 216: 0.9001203981350013, 217: 0.8998982190186363, 218: 0.001019554770536609, 219: 0.007433253926675694, 220: 0.0019372245795278016, 221: 0.002991301616507839, 222: 0.9001349789184026, 223: 0.8996599582406581, 224: 0.0021126500353379563, 225: 0.008756672816910904, 226: 0.0005999999999999894, 227: 10.0, 228: 0.12854030501089322, 229: 1.5789473684191258e-05, 230: 1.797785128725209e-05, 231: 8.23076923076923, 232: 0.01694231544977806, 233: 0.0, 234: 0.0, 235: 0.0004999999999999449, 236: 0.0006999999999999229, 237: 0.010604052262828893, 238: 0.4878048780487804, 239: 0.0, 240: 0.0, 241: 0.011780121343032387, 242: 8.450632811634086e-06, 243: 10, 244: 0.0, 245: 0.047619047619047616, 246: 0.0, 247: 0.002032692470568459, 248: 5.882399999990184e-06, 249: 1.463393218638913e-05, 250: 7.99993520057074e-06, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.25834816059906107, 277: 1.0430313923255448, 278: 0.4266840441059503, 279: 0.8168297647953302, 280: 0.9940205110645302, 281: 0.3971482752180271, 282: 0.000983718086622347, 283: 0.18881534941591438, 284: 0.011800000000000033, 285: 0.970952009132961, 286: 0.23350092722700236, 287: 2.2337543978635916, 288: 0.9777377501008312, 289: 0.9924547735835905, 290: 0.9851252776098363, 291: 0.1309761810395732, 292: 5.101268280056943, 293: 0.5235990916344442, 294: 0.04974766115789641, 295: 0.44471926570099146, 296: 0.998839201477994, 297: 0.03557327195908876, 298: 0.9951406626680374, 299: 1.0738430695550483, 300: 0.9992989150716624, 301: 0.6321230180627598, 302: 0.5953916913504904, 303: 1.1945800197961449e-05, 304: 0.5146638392941667, 305: 0.0380845525536309, 306: 0.0, 307: 2.9493423457881523e-05, 308: 0.7973452224136184, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 1.1945800197961449e-05, 312: 0.0, 313: 0.26894548584030337, 314: 0.0, 315: 0.0, 316: 2.737865214593041e-06, 317: 3.09224437825027e-05, 318: 0.0, 319: 2.4356899999966597e-05, 320: 0.0, 321: 0.0, 322: 0.46700443614289033, 323: 1.0029521847745102, 324: 1.1945800197961449e-05, 325: 2.4356899999966597e-05, 326: 4.154973035335784, 327: 0.0, 328: 0.0, 329: 0.0, 330: 0.0040999999999999925, 331: 10.0, 332: 0.0, 333: 0.0, 334: 0.00341872110939902, 335: 0.5778, 336: 0.0, 337: 0.0, 338: 0.006487780297304232, 339: 0.0, 340: 0.00019174356612172163, 341: 0.0022501682226842017, 342: 0.0, 343: 0.0, 344: 0.006976184748616824, 345: 0.0425531914893617, 346: 0.004865947905734201, 347: 0.020057461917927035, 348: 0.0, 349: 0.0, 350: 0.0006000000000000449, 351: 0.0, 352: 0.0, 353: 0.0, 354: 0.0, 355: 0.0, 356: 1.5429, 357: 1.1905201778188326, 358: 6.7812000000833095e-06, 359: 0.0, 360: 0.0, 361: 0.7474000000000001, 362: 0.0, 363: 2.0, 364: 0.0, 365: 1.0, 366: 0.0, 367: 2.0, 368: 0.0, 369: 0.8025401863056405, 370: 1.5, 371: 0.7071, 372: 1.7320254038, 373: 0.25259999999999994, 374: 1.4142, 375: 6.7812000000833095e-06, 376: 10.0, 377: 0.0017131070167465392, 378: 0.004168287667426132, 379: 10.0, 380: 0.02303883455415959, 381: 0.03592775885339674, 382: 0.004175986140380392, 383: 0.0005545231101251979, 384: 0.000412597992023094, 385: 0.0016328954204705558, 386: 0.00045058576148982056, 387: 0.6393156714558591, 388: 0.31466949936606925, 389: 0.002870674556703532, 390: 0.0008344167814797797, 391: 0.00028826751225140865, 392: 0.7886617002166217, 393: 0.31262029144899645, 394: 0.36077916695447954, 395: 4.8642075395247506e-05, 396: 0.0010304882382204188, 397: 0.0010708970123787657, 398: 0.6631824765069777, 399: 0.0002757194554540451, 400: 0.004347280259688986}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.0, 79: 0.0, 80: 0.0, 81: 0.0, 82: 0.0, 83: 0.0, 84: 0.0, 85: 0.0, 86: 6.915669215143584e-05, 87: 0.0, 88: 0.0, 89: 0.0, 90: 0.0, 91: 0.0, 92: 0.0, 93: 0.0, 94: 0.0, 95: 0.0, 96: 0.0, 97: 7.480711679481134e-10, 98: 0.0, 99: 1.3338131396936082e-10, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0010000000000000009, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.09, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.014005602240896359, 161: 0.016722408026755852, 162: 0.0, 163: 0.0, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.013477088948787063, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0050079506900020535, 202: 0.9000326050810861, 203: 0.0037008145159081996, 204: 0.004355903868126497, 205: 0.003983511774317081, 206: 0.899790857127425, 207: 0.9004704527702285, 208: 8.927920118437973, 209: 0.0011148140796962557, 210: 0.0002394825185443977, 211: 0.9016077433184178, 212: 0.002180588921159467, 213: 0.9000347542692952, 214: 0.8997696181148409, 215: 0.004550314182209536, 216: 0.9001203981350013, 217: 0.8998982190186363, 218: 0.001019554770536609, 219: 0.007433253926675694, 220: 0.0019372245795278016, 221: 0.002991301616507839, 222: 0.9001349789184026, 223: 0.8996599582406581, 224: 0.0021126500353379563, 225: 0.008756672816910904, 226: 0.0, 227: 10.0, 228: 0.12854030501089322, 229: 0.0, 230: 0.0, 231: 8.23076923076923, 232: 0.01694231544977806, 233: 0.0, 234: 0.0, 235: 0.0, 236: 0.0, 237: 0.010604052262828893, 238: 0.4878048780487804, 239: 0.0, 240: 0.0, 241: 0.011780121343032387, 242: 0.0, 243: 10, 244: 0.0, 245: 0.047619047619047616, 246: 0.0, 247: 0.002032692470568459, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.25834816059906107, 277: 1.0430313923255448, 278: 0.4266840441059503, 279: 0.8168297647953302, 280: 0.9940205110645302, 281: 0.3971482752180271, 282: 0.000983718086622347, 283: 0.18881534941591438, 284: 0.011800000000000033, 285: 0.970952009132961, 286: 0.23350092722700236, 287: 2.2337543978635916, 288: 0.9777377501008312, 289: 0.9924547735835905, 290: 0.9851252776098363, 291: 0.1309761810395732, 292: 5.101268280056943, 293: 0.5235990916344442, 294: 0.04974766115789641, 295: 0.44471926570099146, 296: 0.998839201477994, 297: 0.03557327195908876, 298: 0.9951406626680374, 299: 1.0738430695550483, 300: 0.9992989150716624, 301: 0.6321230180627598, 302: 0.5953916913504904, 303: 0.0, 304: 0.5146638392941667, 305: 0.0380845525536309, 306: 0.0, 307: 0.0, 308: 0.7973452224136184, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 0.0, 312: 0.0, 313: 0.26894548584030337, 314: 0.0, 315: 0.0, 316: 0.0, 317: 0.0, 318: 0.0, 319: 0.0, 320: 0.0, 321: 0.0, 322: 0.46700443614289033, 323: 1.0029521847745102, 324: 0.0, 325: 0.0, 326: 4.154973035335784, 327: 0.0, 328: 0.0, 329: 0.0, 330: 0.0040999999999999925, 331: 10.0, 332: 0.0, 333: 0.0, 334: 0.00341872110939902, 335: 0.5778, 336: 0.0, 337: 0.0, 338: 0.006487780297304232, 339: 0.0, 340: 0.00019174356612172163, 341: 0.0022501682226842017, 342: 0.0, 343: 0.0, 344: 0.006976184748616824, 345: 0.0425531914893617, 346: 0.004865947905734201, 347: 0.020057461917927035, 348: 0.0, 349: 0.0, 350: 0.0, 351: 0.0, 352: 0.0, 353: 0.0, 354: 0.0, 355: 0.0, 356: 1.5429, 357: 1.1905201778188326, 358: 0.0, 359: 0.0, 360: 0.0, 361: 0.7474000000000001, 362: 0.0, 363: 2.0, 364: 0.0, 365: 1.0, 366: 0.0, 367: 2.0, 368: 0.0, 369: 0.8025401863056405, 370: 1.5, 371: 0.7071, 372: 1.7320254038, 373: 0.25259999999999994, 374: 1.4142, 375: 0.0, 376: 10.0, 377: 0.0017131070167465392, 378: 0.004168287667426132, 379: 10.0, 380: 0.02303883455415959, 381: 0.03592775885339674, 382: 0.004175986140380392, 383: 0.0005545231101251979, 384: 0.000412597992023094, 385: 0.0016328954204705558, 386: 0.00045058576148982056, 387: 0.6393156714558591, 388: 0.31466949936606925, 389: 0.002870674556703532, 390: 0.0008344167814797797, 391: 0.00028826751225140865, 392: 0.7886617002166217, 393: 0.31262029144899645, 394: 0.36077916695447954, 395: 0.0, 396: 0.0010304882382204188, 397: 0.0010708970123787657, 398: 0.6631824765069777, 399: 0.0, 400: 0.004347280259688986}</t>
         </is>
       </c>
     </row>
@@ -703,7 +703,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 3.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 3.4, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.10559662090813093, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 4.136690647482014, 70: 0.0, 71: 0.0, 72: 0.0, 73: 1.4149659863945578, 74: 0.0, 75: 0.0, 76: 3.4873287371326036e-07, 77: 0.0, 78: 0.0, 79: 0.0, 80: 1.5865532587269627e-09, 81: 1.0083483824328928e-10, 82: 0.0, 83: 0.0, 84: 0.0, 85: 0.0, 86: 0.0, 87: 0.0, 88: 0.0, 89: 7.943426310259696e-11, 92: 6.0434690320118976e-06, 93: 9.000000008838883, 95: 0.0, 96: 0.0, 98: 9.79826812653991e-08, 99: 1.3338131396936082e-11, 100: 9.328129583895494e-07, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.17, 138: 0.0, 139: 2.0381036774479395, 140: 0.0, 141: 0.0, 142: 2.1904761904761907, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.007680491551459293, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.004553734061930784, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.9899874843554443, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0, 202: 8.99640143942423, 203: 0.00016153414743356033, 204: 0.0, 206: 0.0, 207: 0.003728629717653877, 213: 0.0, 214: 0.0, 216: 7.082593198802762e-05, 217: 0.0, 218: 0.0, 219: 0.0, 220: 0.0, 221: 0.0, 222: 0.0, 223: 0.0, 224: 0.0, 225: 0.0, 226: 2.8915662650591534e-05, 227: 1.886756853644063e-05, 228: 0.12854030501089322, 229: 0.00029999999999996696, 230: 0.0, 231: 0.0, 232: 7.11861993686498e-05, 233: 0.0, 239: 8.076892011952911e-05, 240: 0.0, 241: 0.011749591464339995, 242: 9.295696092714932e-05, 244: 0.0, 245: 0.0, 246: 0.0, 248: 0.1647, 249: 1.463393218638913e-05, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 277: 0.3761669604062331, 284: 0.22040000000000004, 285: 0.6446764331523566, 286: 0.6588538431483364, 287: 0.39614418634224924, 288: 0.39881243874977457, 289: 0.4886713834459026, 290: 0.37939526302243487, 291: 0.24827176957219596, 292: 6.2746214572279015, 293: 0.403449334069846, 294: 0.5480528480392896, 295: 0.6235862419801165, 296: 10.0, 297: 0.7003441236189412, 298: 0.6305406791364982, 299: 0.829688382564698, 304: 0.5146638392941667, 305: 0.009065613499685843, 306: 0.0, 307: 0.0004774789113481002, 309: 0.6321177658060569, 310: 0.6321230180627598, 312: 0.0, 313: 10, 314: 0.0, 315: 0.0, 316: 2.1864983372539375, 317: 0.00031650030695070194, 318: 0.0, 319: 2.0015859240496425e-05, 320: 0.0, 321: 0.0, 322: 0.46696240952603324, 323: 10, 324: 5.379319094524265e-06, 325: 2.0015859240496425e-05, 326: 0.0, 327: 0.0, 328: 0.0, 329: 1.562524414433395e-05, 330: 9.999999999998899e-05, 331: 0.00029999999999996696, 332: 0.0, 333: 0.0, 334: 0.0016612095531586832, 335: 0.0, 336: 0.0, 337: 0.0, 338: 3.418736587880217e-05, 339: 0.0, 340: 1.5637543159249456e-05, 341: 2.227221096235431e-05, 342: 0.0, 343: 0.0, 344: 0.097907144575415, 345: 0.0, 346: 9.541074324963704e-05, 347: 0.0, 348: 0.3137, 349: 0.0, 350: 0.0494, 351: 0.0, 352: 0.0038000000000000256, 353: 2.7071, 354: 0.0, 355: 2.7071, 356: 1.2071, 358: 1.2929, 359: 2.0, 360: 0.0, 361: 0.4226000000000002, 362: 0.0, 363: 0.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 1.0, 368: 0.0, 370: 0.0, 371: 6.7812000000833095e-06, 372: 2.5403800000045607e-05, 373: 0.5774, 374: 6.7812000000833095e-06, 375: 1.2071, 376: 0.0006992211002162298, 377: 0.00045449777995317935, 378: 0.0015561607291725314, 379: 0.0016899379432624099, 380: 0.0007365879608789138, 381: 0.0711913790517812, 382: 0.12775026827155556, 383: 0.00028265691505316236, 384: 0.003652256299760121, 385: 0.000148445038224581, 386: 0.0012015620306398329, 387: 0.0, 388: 0.0022844350021132566, 389: 0.0015234265698029382, 390: 0.0025808705101585568, 391: 0.0010890106018385283, 392: 0.03851640513552065, 393: 0.3441710200714874, 394: 0.0005871382192443306, 395: 0.0008917713822457242, 396: 0.0001776703859001375, 397: 0.00319454024031652, 398: 0.007286485758232352, 399: 0.00017232465965885473, 400: 0.002134184615936405}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 3.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 3.4, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.10559662090813093, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 4.136690647482014, 70: 0.0, 71: 0.0, 72: 0.0, 73: 1.4149659863945578, 74: 0.0, 75: 0.0, 76: 3.4873287371326036e-07, 77: 0.0, 78: 0.0, 79: 0.0, 80: 1.5865532587269627e-09, 81: 1.0083483824328928e-10, 82: 0.0, 83: 0.0, 84: 0.0, 85: 0.0, 86: 0.0, 87: 0.0, 88: 0.0, 89: 7.943426310259696e-11, 92: 6.0434690320118976e-06, 93: 9.000000008838883, 95: 0.0, 96: 0.0, 98: 9.79826812653991e-08, 99: 1.3338131396936082e-11, 100: 9.328129583895494e-07, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.17, 138: 0.0, 139: 2.0381036774479395, 140: 0.0, 141: 0.0, 142: 2.1904761904761907, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.007680491551459293, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.004553734061930784, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.9899874843554443, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0, 202: 8.99640143942423, 203: 0.00016153414743356033, 204: 0.0, 206: 0.0, 207: 0.003728629717653877, 213: 0.0, 214: 0.0, 216: 7.082593198802762e-05, 217: 0.0, 218: 0.0, 219: 0.0, 220: 0.0, 221: 0.0, 222: 0.0, 223: 0.0, 224: 0.0, 225: 0.0, 226: 0.0, 227: 0.0, 228: 0.12854030501089322, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.0, 233: 0.0, 239: 0.0, 240: 0.0, 241: 0.011749591464339995, 242: 0.0, 244: 0.0, 245: 0.0, 246: 0.0, 248: 0.1647, 249: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 277: 0.3761669604062331, 284: 0.22040000000000004, 285: 0.6446764331523566, 286: 0.6588538431483364, 287: 0.39614418634224924, 288: 0.39881243874977457, 289: 0.4886713834459026, 290: 0.37939526302243487, 291: 0.24827176957219596, 292: 6.2746214572279015, 293: 0.403449334069846, 294: 0.5480528480392896, 295: 0.6235862419801165, 296: 10.0, 297: 0.7003441236189412, 298: 0.6305406791364982, 299: 0.829688382564698, 304: 0.5146638392941667, 305: 0.009065613499685843, 306: 0.0, 307: 0.0004774789113481002, 309: 0.6321177658060569, 310: 0.6321230180627598, 312: 0.0, 313: 10, 314: 0.0, 315: 0.0, 316: 2.1864983372539375, 317: 0.00031650030695070194, 318: 0.0, 319: 0.0, 320: 0.0, 321: 0.0, 322: 0.46696240952603324, 323: 10, 324: 0.0, 325: 0.0, 326: 0.0, 327: 0.0, 328: 0.0, 329: 0.0, 330: 0.0, 331: 0.0, 332: 0.0, 333: 0.0, 334: 0.0016612095531586832, 335: 0.0, 336: 0.0, 337: 0.0, 338: 0.0, 339: 0.0, 340: 0.0, 341: 2.227221096235431e-05, 342: 0.0, 343: 0.0, 344: 0.097907144575415, 345: 0.0, 346: 0.0, 347: 0.0, 348: 0.3137, 349: 0.0, 350: 0.0494, 351: 0.0, 352: 0.0038000000000000256, 353: 2.7071, 354: 0.0, 355: 2.7071, 356: 1.2071, 358: 1.2929, 359: 2.0, 360: 0.0, 361: 0.4226000000000002, 362: 0.0, 363: 0.0, 364: 0.0, 365: 0.0, 366: 0.0, 367: 1.0, 368: 0.0, 370: 0.0, 371: 0.0, 372: 0.0, 373: 0.5774, 374: 0.0, 375: 1.2071, 376: 0.0006992211002162298, 377: 0.00045449777995317935, 378: 0.0015561607291725314, 379: 0.0016899379432624099, 380: 0.0007365879608789138, 381: 0.0711913790517812, 382: 0.12775026827155556, 383: 0.00028265691505316236, 384: 0.003652256299760121, 385: 0.0, 386: 0.0012015620306398329, 387: 0.0, 388: 0.0022844350021132566, 389: 0.0015234265698029382, 390: 0.0025808705101585568, 391: 0.0010890106018385283, 392: 0.03851640513552065, 393: 0.3441710200714874, 394: 0.0005871382192443306, 395: 0.0008917713822457242, 396: 0.0, 397: 0.00319454024031652, 398: 0.007286485758232352, 399: 0.0, 400: 0.002134184615936405}</t>
         </is>
       </c>
     </row>
@@ -714,17 +714,17 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6675</v>
       </c>
       <c r="C14" t="n">
-        <v>0.004987531172069825</v>
+        <v>0.002493765586034913</v>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.10559662090813093, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.1111111111111111, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.3339130403337495, 79: 0.0, 80: 1.8088728236441168e-09, 81: 1.0083483824328928e-10, 82: 0.0, 83: 4.8431407238119694e-11, 84: 1.3676635662339353e-10, 85: 0.0, 86: 0.0, 87: 0.0, 88: 8.843568238832642e-08, 89: 1.1347751871799565e-07, 90: 1.4638068482187798e-08, 91: 8.999552875845156, 92: 0.0, 93: 9.000002326941114, 94: 4.778149724210535e-07, 95: 8.999981560535383, 96: 4.67653461942089e-08, 97: 6.732640511533021e-08, 98: 9.000000887955801, 99: 1.3338131396936082e-10, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.016025641025641024, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.022768670309653915, 164: 0.0, 165: 0.011123470522803115, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0010513362529844133, 202: 0.00034525258872499166, 203: 0.8998838776243662, 204: 0.04270905080108001, 205: 0.16360634634315596, 206: 0.0005401256207549502, 207: 0.9003214119831544, 208: 9.001284296098403, 209: 0.001212089456127305, 210: 9.017948555422668, 211: 0.8996986776686995, 212: 9.05981110937965, 213: 8.993595975124068, 214: 0.00019002636995885707, 215: 0.0005991545567576448, 216: 0.003839686250866941, 217: 9.000201440481208, 218: 0.007450184293048533, 219: 0.0017891623167675074, 220: 9.58393581343497, 221: 0.001510579591453374, 222: 0.9999999913596681, 223: 10.0, 224: 9.004283945037868, 225: 9.072625975911274, 226: 1.8750000000011813e-05, 227: 1.8867379860739656e-05, 229: 1.5789473684191258e-05, 230: 1.7977851287421747e-05, 231: 0.0, 232: 3.3898190174644294e-06, 233: 0.0, 234: 4.5454499999986187e-05, 235: 4.871794871796897e-05, 236: 3.333333333332966e-05, 237: 1.9148569495584293e-05, 238: 0.0, 239: 0.0, 240: 3.636363636361217e-05, 242: 8.450632811496482e-06, 243: 0.0, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 5.882399999990184e-06, 249: 0.0, 250: 7.999936000404534e-06, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8197299268300126, 277: 0.43810529254715835, 278: 1.3200500113027778, 279: 0.40442940181002135, 280: 0.8015495123647878, 281: 0.7312315015640065, 282: 0.05924179841192049, 283: 0.8446462594456288, 284: 1.2336282703027013, 285: 0.16075341461036857, 286: 0.723456558079298, 287: 0.39698666864482224, 288: 0.2140000950811225, 289: 0.47990514869960527, 290: 0.4676219150423842, 291: 0.8097417380330398, 292: 2.6444933350588844, 293: 0.44462775425029155, 294: 0.02492957109929358, 295: 0.7125234438611803, 296: 0.31254232690033523, 297: 0.9936172998651905, 298: 0.6625398419999683, 299: 0.7633871391180519, 300: 0.40652949695185625, 301: 0.6321230180627598, 302: 0.40461128559308157, 303: 0.0075105850567920695, 304: 0.05333510044114582, 305: 0.001594650773111524, 306: 0.0, 307: 2.9493423457881523e-05, 308: 6.124238416842839e-05, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 0.0053539157059642245, 312: 0.0, 313: 0.26894548584030337, 314: 0.0, 315: 0.0, 316: 9.36822999010763e-06, 317: 2.9491697419365663e-05, 318: 0.0, 319: 0.00041566490153288616, 320: 0.0, 321: 0.0, 322: 0.4669203829091758, 323: 0.12346057763947928, 324: 0.0075105850567920695, 325: 0.00041566490153288616, 326: 1.2625544435799056, 327: 0.004595588235294118, 328: 0.0, 329: 1.562524414433395e-05, 330: 0.021100000000000008, 331: 0.0, 332: 0.0, 333: 6.9300411522633745, 334: 0.0008667180277348815, 335: 2.2222222222367805e-05, 336: 0.0, 337: 0.0032127481847972757, 338: 8.188460569424636e-05, 339: 0.0, 340: 0.14736705228428304, 341: 2.2496957821583182e-07, 342: 0.0, 343: 0.0, 344: 0.23776650200558305, 345: 0.058027079303675046, 346: 0.21739035916706423, 347: 0.6293615944778735, 348: 2.5490196078448157e-05, 349: 0.0, 350: 0.0012999999999999678, 351: 0.0, 352: 0.7474000000000001, 353: 0.20709999999999995, 354: 0.29290000000000005, 355: 0.965919045102521, 356: 1.4571, 357: 0.9305467351769529, 358: 0.20709999999999995, 359: 0.0, 360: 0.0, 361: 2.0406, 362: 0.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 0.0, 367: 1.5, 368: 0.0, 369: 0.5443681080769008, 370: 0.0, 371: 0.0, 372: 1.7320254038, 373: 0.02290000000000003, 374: 1.4142067811865473, 375: 1.4142067811865473, 376: 0.003442769565995084, 377: 0.0011537251337271819, 378: 0.005113099538709552, 379: 0.015763519503546024, 380: 0.00038875475713058327, 381: 0.0014461083617199597, 382: 0.0016979986097345754, 383: 0.0015886337749535647, 384: 0.0026742462445942133, 385: 0.000593780152898324, 386: 0.0021243331676179364, 387: 0.0, 388: 0.0011536396760672687, 389: 0.0004559916263356309, 390: 0.002231579764422767, 391: 0.0010890106018385283, 392: 0.00017963755481582825, 393: 0.0005499037668408948, 394: 0.0004144505077018263, 395: 0.0005026347790840322, 396: 0.0001776703859001375, 397: 0.0030130322721166557, 398: 0.08252310006848626, 399: 0.00010339479579534345, 400: 0.0024605893219032224}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 0.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.0, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.0, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.10559662090813093, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.0, 67: 0.0, 68: 0.0, 69: 0.0, 70: 0.1111111111111111, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.3339130403337495, 79: 0.0, 80: 1.8088728236441168e-09, 81: 1.0083483824328928e-10, 82: 0.0, 83: 4.8431407238119694e-11, 84: 1.3676635662339353e-10, 85: 0.0, 86: 0.0, 87: 0.0, 88: 8.843568238832642e-08, 89: 1.1347751871799565e-07, 90: 1.4638068482187798e-08, 91: 8.999552875845156, 92: 0.0, 93: 9.000002326941114, 94: 4.778149724210535e-07, 95: 8.999981560535383, 96: 4.67653461942089e-08, 97: 6.732640511533021e-08, 98: 9.000000887955801, 99: 1.3338131396936082e-10, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 0.0, 121: 0.0, 122: 0.0, 123: 0.0, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.0, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.016025641025641024, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.0, 161: 0.0, 162: 0.0, 163: 0.022768670309653915, 164: 0.0, 165: 0.011123470522803115, 166: 0.0, 167: 0.0, 168: 0.0, 169: 0.0, 170: 0.0, 171: 0.0, 172: 0.0, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0010513362529844133, 202: 0.00034525258872499166, 203: 0.8998838776243662, 204: 0.04270905080108001, 205: 0.16360634634315596, 206: 0.0005401256207549502, 207: 0.9003214119831544, 208: 9.001284296098403, 209: 0.001212089456127305, 210: 9.017948555422668, 211: 0.8996986776686995, 212: 9.05981110937965, 213: 8.993595975124068, 214: 0.00019002636995885707, 215: 0.0005991545567576448, 216: 0.003839686250866941, 217: 9.000201440481208, 218: 0.007450184293048533, 219: 0.0017891623167675074, 220: 9.58393581343497, 221: 0.001510579591453374, 222: 0.9999999913596681, 223: 10.0, 224: 9.004283945037868, 225: 9.072625975911274, 226: 0.0, 227: 0.0, 229: 0.0, 230: 0.0, 231: 0.0, 232: 0.0, 233: 0.0, 234: 0.0, 235: 0.0, 236: 0.0, 237: 0.0, 238: 0.0, 239: 0.0, 240: 0.0, 241: 0.0, 242: 0.0, 243: 0.0, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.0, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8197299268300126, 277: 0.43810529254715835, 278: 1.3200500113027778, 279: 0.40442940181002135, 280: 0.8015495123647878, 281: 0.7312315015640065, 282: 0.05924179841192049, 283: 0.8446462594456288, 284: 1.2336282703027013, 285: 0.16075341461036857, 286: 0.723456558079298, 287: 0.39698666864482224, 288: 0.2140000950811225, 289: 0.47990514869960527, 290: 0.4676219150423842, 291: 0.8097417380330398, 292: 2.6444933350588844, 293: 0.44462775425029155, 294: 0.02492957109929358, 295: 0.7125234438611803, 296: 0.31254232690033523, 297: 0.9936172998651905, 298: 0.6625398419999683, 299: 0.7633871391180519, 300: 0.40652949695185625, 301: 0.6321230180627598, 302: 0.40461128559308157, 303: 0.0075105850567920695, 304: 0.05333510044114582, 305: 0.001594650773111524, 306: 0.0, 307: 0.0, 308: 0.0, 309: 0.7293273785356611, 310: 0.6321230180627598, 311: 0.0053539157059642245, 312: 0.0, 313: 0.26894548584030337, 314: 0.0, 315: 0.0, 316: 0.0, 317: 0.0, 318: 0.0, 319: 0.0, 320: 0.0, 321: 0.0, 322: 0.4669203829091758, 323: 0.12346057763947928, 324: 0.0075105850567920695, 325: 0.0, 326: 1.2625544435799056, 327: 0.004595588235294118, 328: 0.0, 329: 0.0, 330: 0.021100000000000008, 331: 0.0, 332: 0.0, 333: 6.9300411522633745, 334: 0.0008667180277348815, 335: 0.0, 336: 0.0, 337: 0.0032127481847972757, 338: 0.0, 339: 0.0, 340: 0.14736705228428304, 341: 0.0, 342: 0.0, 343: 0.0, 344: 0.23776650200558305, 345: 0.058027079303675046, 346: 0.21739035916706423, 347: 0.6293615944778735, 348: 0.0, 349: 0.0, 350: 0.0012999999999999678, 351: 0.0, 352: 0.7474000000000001, 353: 0.20709999999999995, 354: 0.29290000000000005, 355: 0.965919045102521, 356: 1.4571, 357: 0.9305467351769529, 358: 0.20709999999999995, 359: 0.0, 360: 0.0, 361: 2.0406, 362: 0.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 0.0, 367: 1.5, 368: 0.0, 369: 0.5443681080769008, 370: 0.0, 371: 0.0, 372: 1.7320254038, 373: 0.02290000000000003, 374: 1.4142067811865473, 375: 1.4142067811865473, 376: 0.003442769565995084, 377: 0.0011537251337271819, 378: 0.005113099538709552, 379: 0.015763519503546024, 380: 0.00038875475713058327, 381: 0.0014461083617199597, 382: 0.0016979986097345754, 383: 0.0015886337749535647, 384: 0.0026742462445942133, 385: 0.000593780152898324, 386: 0.0021243331676179364, 387: 0.0, 388: 0.0011536396760672687, 389: 0.0004559916263356309, 390: 0.002231579764422767, 391: 0.0010890106018385283, 392: 0.00017963755481582825, 393: 0.0005499037668408948, 394: 0.0004144505077018263, 395: 0.0005026347790840322, 396: 0.0, 397: 0.0030130322721166557, 398: 0.08252310006848626, 399: 0.0, 400: 0.0024605893219032224}</t>
         </is>
       </c>
     </row>
@@ -745,7 +745,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 1.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.13333333333333333, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.16393442622950818, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.12224938875305623, 67: 0.0, 68: 3.816793893129771, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.014193241159702325, 79: 0.2463342280155607, 80: 8.88257610756951e-07, 81: 9.982648986085639e-10, 82: 0.0, 83: 2.440458610728851e-07, 84: 6.838317831169677e-10, 85: 0.4679940636032788, 86: 0.0, 87: 0.0, 88: 0.0, 89: 1.1000151539382073, 90: 2.1300225196379494, 91: 0.0003803509547799874, 92: 0.0, 93: 8.59866087701943e-05, 94: 0.0, 95: 0.25329102060355047, 96: 1.402726559095296, 97: 0.0, 98: 6.123916354303928, 99: 1.3338131396936082e-10, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 2.0, 121: 0.0, 122: 0.0, 123: 1.5, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.014005602240896359, 161: 0.008361204013377926, 162: 0.04887218045112782, 163: 0.0, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.01212856276531231, 169: 0.0, 170: 0.02932551319648094, 171: 0.0, 172: 0.2127659574468085, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0028176264184765236, 202: 0.9000390071273964, 203: 0.0012570070444007878, 204: 0.003768864850997538, 205: 0.007213951926232086, 206: 1.0387031168364427e-06, 207: 10.0, 208: 0.0019318652240808197, 209: 0.0014616022214632388, 210: 0.899117747696819, 211: 0.9038249825326757, 212: 0.8996966572911498, 213: 0.8971243156728078, 214: 8.848637160944888, 215: 0.900134847160709, 216: 0.02256863223331397, 217: 0.8999922086925541, 218: 0.02907849159776472, 219: 0.02193564284713709, 220: 0.0013374900039583972, 221: 0.9000582585100942, 222: 0.8987362128773716, 223: 0.899569374331416, 224: 0.0017393643468515394, 225: 0.9014604804546386, 226: 9.787234042554771e-05, 227: 0.037754004641421854, 228: 0.0034990427015250377, 229: 1.5789473684191258e-05, 230: 1.797785128725209e-05, 231: 3.230769230769231, 232: 0.7627126687706143, 233: 0.0, 234: 0.0, 235: 0.002515384615384586, 236: 2.3333, 237: 0.0052708659416277, 238: 0.19512195121951217, 239: 0.0, 240: 0.0035999999999999366, 241: 1.5247292017422574e-05, 242: 8.450632811634086e-06, 243: 0.012969910897608256, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.001933641778146534, 248: 5.882352941161129e-06, 249: 1.463393218638913e-05, 250: 1.0799913600761947e-05, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8243334892350003, 277: 0.204547437485822, 278: 0.47975128307457876, 279: 0.8609864371029848, 280: 0.8392184263333812, 281: 0.8193946899498071, 282: 0.6810087247520019, 283: 0.9992436374579663, 284: 1.1753999999999998, 285: 0.2677413506103977, 286: 0.4189463276854342, 287: 0.5445508880505275, 288: 0.653876033921316, 289: 0.7013644051318362, 290: 0.5166322850745407, 291: 0.7996632222492287, 292: 1.906043742720331, 293: 0.45583993125882266, 294: 0.8194007140812607, 295: 0.9112385813960627, 296: 0.9894209423343474, 297: 0.9194416935455614, 298: 0.6082789072442476, 299: 0.4516424156118982, 300: 0.945391234185834, 301: 0.5000036787698194, 302: 0.40461128559308157, 303: 0.025911589482746796, 304: 0.5146638392941667, 305: 0.8942554528318822, 306: 0.0, 307: 0.27327709692821894, 308: 6.12423759331812e-05, 309: 0.6321180132629585, 310: 0.26424603612551967, 311: 0.02594015796220097, 312: 0.0, 313: 0.4621197859236748, 314: 0.0, 315: 0.0, 316: 0.0002450557514834778, 317: 0.8571387644664742, 318: 0.0, 319: 1.2217340668482244, 320: 0.0, 321: 0.0, 322: 0.46700443614289033, 323: 1.1913485559013017, 324: 0.025911589482746796, 325: 1.2217340668482244, 326: 0.2806292649334156, 327: 0.0, 328: 0.0, 329: 6.03135986499789, 330: 10.0, 331: 0.0006000000000000449, 332: 0.0, 333: 0.1646090534979424, 334: 0.013602657935285, 335: 0.0, 336: 0.8333333333333334, 337: 0.007710595643513461, 338: 0.004787100025195156, 339: 0.3333333333333333, 340: 0.0008132571942405459, 341: 0.03937254457310579, 342: 0.0, 343: 0.0, 344: 0.097907144575415, 345: 0.009671179883945842, 346: 0.008627857074706638, 347: 0.011438174228871903, 348: 0.00208947368421053, 349: 0.0, 350: 0.0006388888888887445, 351: 0.5, 352: 0.4226, 353: 1.4142067811999999, 354: 0.20709999999999995, 355: 0.20709999999999995, 356: 1.2929, 357: 2.732001616534842, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 0.4226, 362: 0.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 1.5, 367: 1.0, 368: 0.0, 369: 0.4226661278217193, 370: 1.5, 371: 0.29290000000000005, 372: 2.5403800000045607e-05, 373: 1.4225999999999999, 374: 1.2929, 375: 1.4142067811999999, 376: 0.1606094606240955, 377: 0.21564870817746395, 378: 0.06074584560662478, 379: 0.08059064716312062, 380: 0.3298481810369521, 381: 0.10000642714827433, 382: 10.0, 383: 0.7002577783106528, 384: 0.36181787619003963, 385: 0.13712610405997178, 386: 0.08513667768098528, 387: 0.0034050328045841464, 388: 0.7715564997886898, 389: 0.7617858290238669, 390: 0.0017076436458191681, 391: 0.10688318759809098, 392: 0.04718127542663923, 393: 0.10571899917514445, 394: 0.35939766526213995, 395: 0.08705310093230632, 396: 0.3869305664131902, 397: 0.002051040040657841, 398: 0.14841302810180873, 399: 0.37308288816129587, 400: 0.08549651177388408}</t>
+          <t>{0: 0.0, 1: 0.0, 2: 0.0, 3: 0.0, 4: 0.0, 5: 0.0, 6: 0.0, 7: 0.0, 8: 0.0, 9: 0.0, 10: 0.0, 11: 0.0, 12: 0.0, 13: 0.0, 14: 0.0, 15: 0.0, 16: 0.0, 17: 0.0, 18: 0.0, 19: 0.0, 20: 0.0, 21: 1.0, 22: 0.0, 23: 0.0, 24: 0.0, 25: 0.0, 26: 0.0, 27: 0.0, 28: 0.0, 29: 0.0, 30: 0.0, 31: 0.0, 32: 0.0, 33: 0.0, 34: 0.0, 35: 0.0, 36: 0.0, 37: 0.13333333333333333, 38: 0.0, 39: 0.0, 40: 0.0, 41: 0.0, 42: 0.0, 43: 0.0, 44: 0.0, 45: 0.0, 46: 0.0, 47: 0.0, 48: 0.0, 49: 0.0, 50: 0.16393442622950818, 51: 0.0, 52: 0.0, 53: 0.0, 54: 0.0, 55: 0.0, 56: 0.0, 57: 0.0, 58: 0.0, 59: 0.0, 60: 0.0, 61: 0.0, 62: 0.0, 63: 0.0, 64: 0.0, 65: 0.0, 66: 0.12224938875305623, 67: 0.0, 68: 3.816793893129771, 69: 0.0, 70: 0.0, 71: 0.0, 72: 0.0, 73: 0.0, 74: 0.0, 75: 0.0, 76: 0.0, 77: 0.0, 78: 0.014193241159702325, 79: 0.2463342280155607, 80: 8.88257610756951e-07, 81: 9.982648986085639e-10, 82: 0.0, 83: 2.440458610728851e-07, 84: 6.838317831169677e-10, 85: 0.4679940636032788, 86: 0.0, 87: 0.0, 88: 0.0, 89: 1.1000151539382073, 90: 2.1300225196379494, 91: 0.0003803509547799874, 92: 0.0, 93: 8.59866087701943e-05, 94: 0.0, 95: 0.25329102060355047, 96: 1.402726559095296, 97: 0.0, 98: 6.123916354303928, 99: 1.3338131396936082e-10, 100: 0.0, 101: 0.0, 102: 0.0, 103: 0.0, 104: 0.0, 105: 0.0, 106: 0.0, 107: 0.0, 108: 0.0, 109: 0.0, 110: 0.0, 111: 0.0, 112: 0.0, 113: 0.0, 114: 0.0, 115: 0.0, 116: 0.0, 117: 0.0, 118: 0.0, 119: 0.0, 120: 2.0, 121: 0.0, 122: 0.0, 123: 1.5, 124: 0.0, 125: 0.0, 126: 0.0, 127: 0.0, 128: 0.0, 129: 0.0, 130: 0.0, 131: 0.076, 132: 0.0, 133: 0.0, 134: 0.0, 135: 0.0, 136: 0.0, 137: 0.0, 138: 0.0, 139: 0.0, 140: 0.0, 141: 0.0, 142: 0.0, 143: 0.0, 144: 0.0, 145: 0.0, 146: 0.0, 147: 0.0, 148: 0.0, 149: 0.0, 150: 0.0, 151: 0.0, 152: 0.0, 153: 0.0, 154: 0.0, 155: 0.0, 156: 0.0, 157: 0.0, 158: 0.0, 159: 0.0, 160: 0.014005602240896359, 161: 0.008361204013377926, 162: 0.04887218045112782, 163: 0.0, 164: 0.0, 165: 0.0, 166: 0.0, 167: 0.0, 168: 0.01212856276531231, 169: 0.0, 170: 0.02932551319648094, 171: 0.0, 172: 0.2127659574468085, 173: 0.0, 174: 0.0, 175: 0.0, 176: 0.0, 177: 0.0, 178: 0.0, 179: 0.0, 180: 0.0, 181: 0.0, 182: 0.0, 183: 0.0, 184: 0.0, 185: 0.0, 186: 0.0, 187: 0.0, 188: 0.0, 189: 0.0, 190: 0.0, 191: 0.0, 192: 0.0, 193: 0.0, 194: 0.0, 195: 0.0, 196: 0.0, 197: 0.0, 198: 0.0, 199: 0.0, 200: 0.0, 201: 0.0028176264184765236, 202: 0.9000390071273964, 203: 0.0012570070444007878, 204: 0.003768864850997538, 205: 0.007213951926232086, 206: 1.0387031168364427e-06, 207: 10.0, 208: 0.0019318652240808197, 209: 0.0014616022214632388, 210: 0.899117747696819, 211: 0.9038249825326757, 212: 0.8996966572911498, 213: 0.8971243156728078, 214: 8.848637160944888, 215: 0.900134847160709, 216: 0.02256863223331397, 217: 0.8999922086925541, 218: 0.02907849159776472, 219: 0.02193564284713709, 220: 0.0013374900039583972, 221: 0.9000582585100942, 222: 0.8987362128773716, 223: 0.899569374331416, 224: 0.0017393643468515394, 225: 0.9014604804546386, 226: 0.0, 227: 0.037754004641421854, 228: 0.0034990427015250377, 229: 0.0, 230: 0.0, 231: 3.230769230769231, 232: 0.7627126687706143, 233: 0.0, 234: 0.0, 235: 0.002515384615384586, 236: 2.3333, 237: 0.0052708659416277, 238: 0.19512195121951217, 239: 0.0, 240: 0.0035999999999999366, 241: 0.0, 242: 0.0, 243: 0.012969910897608256, 244: 0.0, 245: 0.0, 246: 0.0, 247: 0.001933641778146534, 248: 0.0, 249: 0.0, 250: 0.0, 251: 0.0, 252: 0.0, 253: 0.0, 254: 0.0, 255: 0.0, 256: 0.0, 257: 0.0, 258: 0.0, 259: 0.0, 260: 0.0, 261: 0.0, 262: 0.0, 263: 0.0, 264: 0.0, 265: 0.0, 266: 0.0, 267: 0.0, 268: 0.0, 269: 0.0, 270: 0.0, 271: 0.0, 272: 0.0, 273: 0.0, 274: 0.0, 275: 0.0, 276: 0.8243334892350003, 277: 0.204547437485822, 278: 0.47975128307457876, 279: 0.8609864371029848, 280: 0.8392184263333812, 281: 0.8193946899498071, 282: 0.6810087247520019, 283: 0.9992436374579663, 284: 1.1753999999999998, 285: 0.2677413506103977, 286: 0.4189463276854342, 287: 0.5445508880505275, 288: 0.653876033921316, 289: 0.7013644051318362, 290: 0.5166322850745407, 291: 0.7996632222492287, 292: 1.906043742720331, 293: 0.45583993125882266, 294: 0.8194007140812607, 295: 0.9112385813960627, 296: 0.9894209423343474, 297: 0.9194416935455614, 298: 0.6082789072442476, 299: 0.4516424156118982, 300: 0.945391234185834, 301: 0.5000036787698194, 302: 0.40461128559308157, 303: 0.025911589482746796, 304: 0.5146638392941667, 305: 0.8942554528318822, 306: 0.0, 307: 0.27327709692821894, 308: 0.0, 309: 0.6321180132629585, 310: 0.26424603612551967, 311: 0.02594015796220097, 312: 0.0, 313: 0.4621197859236748, 314: 0.0, 315: 0.0, 316: 0.0002450557514834778, 317: 0.8571387644664742, 318: 0.0, 319: 1.2217340668482244, 320: 0.0, 321: 0.0, 322: 0.46700443614289033, 323: 1.1913485559013017, 324: 0.025911589482746796, 325: 1.2217340668482244, 326: 0.2806292649334156, 327: 0.0, 328: 0.0, 329: 6.03135986499789, 330: 10.0, 331: 0.0, 332: 0.0, 333: 0.1646090534979424, 334: 0.013602657935285, 335: 0.0, 336: 0.8333333333333334, 337: 0.007710595643513461, 338: 0.004787100025195156, 339: 0.3333333333333333, 340: 0.0008132571942405459, 341: 0.03937254457310579, 342: 0.0, 343: 0.0, 344: 0.097907144575415, 345: 0.009671179883945842, 346: 0.008627857074706638, 347: 0.011438174228871903, 348: 0.00208947368421053, 349: 0.0, 350: 0.0, 351: 0.5, 352: 0.4226, 353: 1.4142067811999999, 354: 0.20709999999999995, 355: 0.20709999999999995, 356: 1.2929, 357: 2.732001616534842, 358: 0.29290000000000005, 359: 2.0, 360: 0.0, 361: 0.4226, 362: 0.0, 363: 2.0, 364: 0.0, 365: 2.5, 366: 1.5, 367: 1.0, 368: 0.0, 369: 0.4226661278217193, 370: 1.5, 371: 0.29290000000000005, 372: 0.0, 373: 1.4225999999999999, 374: 1.2929, 375: 1.4142067811999999, 376: 0.1606094606240955, 377: 0.21564870817746395, 378: 0.06074584560662478, 379: 0.08059064716312062, 380: 0.3298481810369521, 381: 0.10000642714827433, 382: 10.0, 383: 0.7002577783106528, 384: 0.36181787619003963, 385: 0.13712610405997178, 386: 0.08513667768098528, 387: 0.0034050328045841464, 388: 0.7715564997886898, 389: 0.7617858290238669, 390: 0.0017076436458191681, 391: 0.10688318759809098, 392: 0.04718127542663923, 393: 0.10571899917514445, 394: 0.35939766526213995, 395: 0.08705310093230632, 396: 0.3869305664131902, 397: 0.002051040040657841, 398: 0.14841302810180873, 399: 0.37308288816129587, 400: 0.08549651177388408}</t>
         </is>
       </c>
     </row>

</xml_diff>